<commit_message>
Created example Audit Dashboard (with search) using dummy data
</commit_message>
<xml_diff>
--- a/dashboard/DummyData.xlsx
+++ b/dashboard/DummyData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\2015-2019 - Master of Data Science\2019-S2 - Capstone Professional Project\Dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\2015-2019 - Master of Data Science\2019-S2 - Capstone Professional Project\Project Code\dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47EB867-FE55-4CB9-8624-1C4D3E6D535F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA128D7C-7535-4FDB-98B4-1F63CA3236C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3927FDB-01BF-4B08-B8D1-941CE14D3EB4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Bills</t>
   </si>
   <si>
-    <t>STATUTES AMENDMENT (DECRIMINALISATION OF SEX WORK) BILL</t>
-  </si>
-  <si>
     <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-10-26906</t>
   </si>
   <si>
@@ -85,13 +82,630 @@
   </si>
   <si>
     <t>Fire and Emergency Services (Volunteer Charters) Amendment Bill</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>The Hon. V.A. CHAPMAN (Bragg—Deputy Premier, Attorney-General) (12:11): Obtained leave and introduced a bill for an act to amend, recognise and regulate certain forms of surrogacy in South Australia, to ensure commercial surrogacy remains unlawful in South Australia and to make related amendments to the Assisted Reproductive Treatment Act 1988, the Births, Deaths and Marriages Registration Act 1996 and the Family Relationships Act 1975, and for other purposes. Read a first time.
+Second Reading
+The Hon. V.A. CHAPMAN (Bragg—Deputy Premier, Attorney-General) (12:12): I move:
+That this bill be now read a second time.
+The Surrogacy Bill 2019 repeals part 2B of the Family Relationships Act 1975 and creates a standalone act to recognise and regulate certain forms of surrogacy in South Australia. Part 2B of the act has been the subject of considerable discussion over recent years and involves an extremely sensitive area of policy for the community. The bill now before the parliament can be traced to the Family Relationships (Surrogacy)Amendment Act 2015, as introduced by the Hon. John Dawkins MLC in late 2014, which commenced on assent in 2015 and reformed the area of surrogacy through amendments to the Family Relationships Act.
+On 26 December 2017, the South Australian Law Reform Institute was asked by the former attorney-general to inquire into and report on the law regulating surrogacy in South Australia, contained in part 2B of the Family Relationships Act, and to suggest a suitable regulatory framework for surrogacy in South Australia. I supported the SALRI undertaking this reference.
+Referral of surrogacy to the SALRI for proper investigation and recommendations for reform based on best practice in this area and with the guidance of other jurisdictions was considered a suitable way to achieve effective, modern and appropriate reform of surrogacy in South Australia. The SALRI presented the government with its report on 30 October 2018. That report made 69 recommendations, including a recommendation for a standalone surrogacy act.
+I take this opportunity to thank the SALRI and, in particular, Professor John Williams, Dr David Plater, Dr Sarah Moulds, Ms Madeleine Thompson, Anita Brunacci, and the entire team of University of Adelaide Law Reform students working on this referral. A draft bill was prepared in accordance with the recommendations of the SALRI and tabled in parliament in late 2018 for an extended period of public consultation.
+This bill before the parliament is the culmination of the work of Mr Dawkins, the SALRI and the government on this important matter of law reform to affected members of the community. The government has considered the SALRI's report and the submissions of both members of the public and stakeholders in order to present a suitable legislative regulatory framework for surrogacy in South Australia.
+Surrogacy—the practice of a woman, (known as the surrogate) becoming pregnant with a child, carrying the pregnancy and giving birth to a child for another person or couple (known as the intending parents)—is a complex and sensitive subject. As noted by the SALRI, surrogacy raises many ethical, legal and other issues and implications. It attracts strong, emotional and often conflicting views from both those directly affected and legal and academic commentators. The development of a complete regulatory framework for surrogacy requires sensitivity and careful consideration to ensure that a moderate and suitable way forward is achieved, giving regard to the resulting impact on South Australian families.
+Commercial surrogacy, where a fee is charged for carrying the pregnancy and delivering the child, will remain unlawful. This is a position reflected in the law regulating surrogacy across Australia. The system provided by the bill will facilitate domestic, non-commercial surrogacy, where no fee is charged but various medical and other costs may be recovered, and will result in an application for transfer of parentage by the Youth Court to intending parents if the parties meet the requirements of the regulatory scheme set out in the bill.
+A standalone act is preferred, on recommendation of the SALRI, after hearing from the community that parties have difficulty navigating the role and content of the legal requirements in part 2B of the Family Relationships Act. However, the new standalone bill retains the appropriate basic structure of the current scheme. The bill sets out what is considered to be a 'lawful surrogacy agreement'.
+A lawful surrogacy agreement is an agreement that complies with the requirements of the legislation but is unenforceable except for its financial aspects. The intending parents under a lawful surrogacy agreement are entitled to apply to the Youth Court for transfer of parentage of the child. Consistent with the current scheme, an order for the transfer of parentage by the Youth Court must be in the best interests of the child born as the result of the surrogacy agreement. The birth mother must also consent to the transfer.
+The lawful practice of surrogacy in South Australia will be guided by the principles set out in the bill, including that the best interests of any child born as a result of a lawful surrogacy agreement is a primary consideration in the administration and operation of the act; and the surrogacy principles as follows:
+that the human rights of all parties to a lawful surrogacy agreement, including any child born as a result of the agreement, must be respected; and
+that the surrogate mother under a lawful surrogacy agreement should not be financially disadvantaged as a result of her involvement.
+Key innovations in the bill adopted from the SALRI report include updating outdated language around surrogacy used in the Family Relationships Act, raising the required age of parties to surrogacy agreements to 25 or older, allowing surrogacy agreements in which neither intending parents provides genetic material, making clearer provision for the payment of reasonable surrogacy costs, including compensating surrogates for loss of income, and providing less complex fertility requirements that include same-sex couples and single intending parents.
+The bill also implements the SALRI recommendation of accommodating cross-jurisdictional service provision by removing the requirements for fertility treatment to take place in South Australia, and allowing interstate lawyers and counsellors to fulfil advisory functions under the bill. Existing protections will continue, including the requirement for parties to obtain counselling from an appropriately qualified counsellor and legal advice from a legal practitioner in order for the agreement to be a lawful surrogacy agreement, that the parties not have impaired decision-making capacity, that the surrogate mother must not be pregnant at the time the agreement is entered into and that the agreement must be in writing.
+The bill ensures that the counsellors have an appropriate role in the surrogacy process to counsel parties to an agreement. The bill brings the counsellor role back to their core function of ensuring that parties have fully considered the issues arising from a surrogacy agreement, and the proposed parentage order. There are strong and conflicting views about the practice of surrogacy in South Australia, across Australia and internationally. Both the SALRI and the government have listened carefully to and considered the views of the community on this important issue.
+Ultimately, there are divergent views and cross-jurisdictional complexities that cannot be resolved by this bill alone. However, it is this government's view that the bill before the parliament strikes an appropriate and suitable balance to properly regulate the practice of non-commercial surrogacy in this state, having regard to the needs of the community and the acknowledgement of the privacy of parties to lawful arrangements within appropriate parameters set by legislation.
+Again, I would like to reflect on the extensive history of this law and thank the Hon. John Dawkins MLC of the other place for his tireless work to assist people in accessing surrogacy in South Australia. I commend the bill for members' consideration, and I hope ultimate approval, and seek leave to have the explanation of clauses inserted without my reading it.
+Leave granted.
+Explanation of Clauses
+Part 1—Preliminary 1—Short title 2—Commencement
+These clauses are formal.
+3—Simplified outline of Act
+This clause provides a simplified outline of the proposed measure.
+4—Interpretation
+This clause defines key terms to be used in the proposed measure.
+5—Interaction with other Acts
+This clause provides that, except where the contrary intention appears, nothing in the measure will limit the operation of any law relating to the guardianship, custody, protection or adoption of children.
+Part 2—Guiding principles for purposes of Act
+6—Best interests of child paramount
+This clause provides that the best interests of any child born as a result of a lawful surrogacy agreement is to be a primary consideration (including for the Court) in respect of the administration and operation of the proposed measure.
+7—Surrogacy principles
+This clause sets out the surrogacy principles which are to inform the Minister, the Court and each person or body engaged in the administration of the proposed measure. The principles are:
+the human rights of all parties to a lawful surrogacy agreement, including any child born as a result of the agreement, must be respected;
+the surrogate mother under a lawful surrogacy agreement should not be financially disadvantaged as a result of her involvement in the lawful surrogacy agreement.
+8—Presumptions under Family Relationships Act 1975 to apply until parentage order made
+The clause provides that presumptions and other rules as to the parentage of a child under the Family Relationships Act 1975 continue to apply to a child born as a result of a surrogacy arrangement until such time as the Court makes an order or orders as to parentage of the child under the proposed measure.
+Part 3—Lawful surrogacy agreements
+Division 1—Lawful surrogacy agreements
+9—Surrogacy agreements not in accordance with Act void and of no effect
+This clause provides that surrogacy agreements other than as provided for in this Act are void and of no effect.
+10—Certain surrogacy agreements lawful in South Australia
+The clause sets out the elements of a lawful surrogacy agreement, namely who may be a party to a lawful surrogacy agreement (including definitions of lawful surrogacy agreement, surrogate mother and intended parent), and the provisions that must be satisfied by a surrogate mother and an intended parent under a lawful surrogacy agreement. It also sets out the requirements with which a lawful surrogacy agreement must comply.
+11—Extent to which surrogacy costs are payable
+This clause provides that no payment of any form may be made in relation to a lawful surrogacy agreement except for matters as provided for in the clause and defined as the reasonable surrogacy costs. A provision in a lawful surrogacy agreement that is inconsistent with the reasonable surrogacy costs as defined is to be void and of no effect. The clause also clarifies that it does not authorise the regulations to allow for commercial surrogacy. The reasonable surrogacy costs include:
+such reasonable costs as may be incurred, or likely to be incurred, in respect of the lawful surrogacy agreement (such as costs relating to the pregnancy that is the subject of the agreement, the birth of the child, medical, counselling or legal services provided in relation to the agreement, reasonable out of pocket expenses incurred by the surrogate mother;
+payments representing loss of income of a kind to be prescribed by the regulations;
+other costs of a kind to be prescribed by the regulations.
+12—Variation of lawful surrogacy agreement
+The clause allows a lawful surrogacy agreement to be varied if in writing and signed by all the parties to the agreement.
+13—Extent to which lawful surrogacy agreement can be enforced
+The clause provides that a provision of a lawful surrogacy agreement relating to the reasonable surrogacy costs is enforceable in a court of competent jurisdiction. This does not apply if the surrogate mother refuses or fails to relinquish the custody or rights to the intended parents in relation to a child born as a result of the lawful surrogacy arrangement or the surrogate mother does not consent to the making of a parentage order in relation to the child. A lawful surrogacy agreement is otherwise not enforceable.
+Division 2—Counselling
+14—Counselling requirements prior to entering lawful surrogacy agreement
+The clause provides that a surrogate mother and the intended parents must each undergo counselling before entering a lawful surrogacy arrangements. The counselling must comply with the requirements set out in the clause. The costs of such counselling are to be met by the intended parents.
+15—Intended parents to ensure counselling available to surrogate mother during pregnancy and after birth
+The clause provides that the intended parents must take reasonable steps to ensure that the surrogate mother and the spouse or domestic partner of the surrogate mother are offered counselling during any period during which the surrogate mother is attempting to become pregnant for the purposes of a lawful surrogacy agreement, or during any pregnancy to which a lawful surrogacy agreement relates. The costs of such counselling are to be met by the intended parents, and it is an offence, with a maximum penalty of $5,000, for the intended parents to refuse or fail to comply with this provision.
+Division 3—Preservation of certain rights of surrogate mother
+16—Rights of surrogate mother to manage pregnancy and birth
+The clause provides that a surrogate mother has the same rights to manager her pregnancy and birth as any other pregnant woman, and that any provision in a lawful surrogacy agreement to the contrary is void.
+17—Medical decisions affecting surrogate mother or child
+The clause provides that for the purposes of the proposed Act, the Consent to Medical Treatment and Palliative Care Act 1995 and any other Act or law, a question relating to any medical treatment to be provided to a surrogate mother, or to an unborn child to which a lawful surrogacy agreement relates, is to be determined as if the lawful surrogacy agreement did not exist. The proposed Act is also not intended to limit the operation of an advanced care directive under the Advance Care Directives Act 2013.
+Part 4—Court orders relating to lawful surrogacy agreements
+18—Court may make orders as to parentage of child born as a result of lawful surrogacy agreement
+This clause provides for the Youth Court to make orders in relation to a child born as a result of a lawful surrogacy agreement. An application for orders must be made by 1 or both of the intended parents not less than 30 days but not more than 12 months after a child is born as a result of the lawful surrogacy agreement (or such later time as the Court may allow if it is in the interests of the child or exceptional circumstances exist).
+The Court may make any of the following orders on application:
+that the relationship between the child and the intended parent or parent is as specified in the order;
+that the relationship between the child and the surrogate mother is as specified in the order;
+that the relationships of all other persons to the child are to be determined according to the other relationships specified in the order;
+that the name of the child is as specified in the order;
+such consequential or ancillary orders as the Court considers appropriate.
+If there is more than 1 child born as a result of the pregnancy, the application will be taken to relate to the child and each of the birth siblings (unless the Court considers it is not in the best interests of the child to do so).
+Before making an order, the Court must be satisfied of a number of matters set out in subclause (4), including that making the order is in the best interests of the child. The Court may make an order where only 1 of the intended parents applies for the order (instead of both) if satisfied that the other intended parent consents, if the other intended parent cannot be contacted to obtain their consent or in other circumstances as prescribed by the regulations.
+The clause makes further provisions about the manner in which the Court may dispense or excuse a failure to comply either with the provisions of the clause or a requirement under proposed Part 3.
+The clause also enables the Court to dispense with certain requirements under Part 3 of the measure, and makes further procedural provision in relation to orders under the proposed section (including provisions revoking existing appointments as guardians and displacing the presumption as to parentage under the Family Relationships Act 1975).
+19—Court may revoke order under section 18
+The clause provides for the circumstances in which the Court may, on the application of the woman who gave birth to a child the subject of a lawful surrogacy agreement, revoke an order made under proposed section 18.
+The clause also requires the Court to make orders declaring the relationship of the child to the birth mother and the intended parents following the revocation.
+20—Court may require separate representation of child
+This clause provides for the Court to order that a child born as a result of a lawful surrogacy agreement be separately represented in proceedings.
+21—Court to notify Registrar of Births, Deaths and Marriages
+This clause requires the Registrar of the Youth Court to give written notice to the Registrar of Births, Deaths and Marriages of the details as provided in the clause of any orders made under proposed section 18 or 19.
+22—Access to Court records
+The clause provides that the records of proceedings relating to an order under proposed section 18 or 19 are not open to inspection.
+Part 5—Offences relating to surrogacy agreements
+23—Offence relating to commercial surrogacy agreements
+The clause provides for an offence with a maximum penalty of imprisonment for 12 months for a person who enters a commercial surrogacy agreement.
+24—Offence to arrange etc surrogacy agreement for another person
+The clause provides for an offence with a maximum penalty of imprisonment for 12 months for a person who for valuable consideration:
+negotiates, or arranges or obtains the benefit of, a surrogacy agreement on behalf of another;
+offers to negotiate, or arrange or obtain the benefit of a surrogacy agreement on behalf of another;
+arranges, or offers to arrange, introductions between people seeking to enter a surrogacy agreement.
+25—Offence to induce person to enter surrogacy agreement
+The clause provides for an offence with a maximum penalty of imprisonment for 5 years for a person who, by threat of harm, or by dishonesty or undue influence, induces another to enter a surrogacy agreement. it also provides an offence with a maximum penalty of imprisonment for 2 years for a person who for valuable consideration, induces another to enter into a surrogacy agreement.
+26—Offence to advertise certain services relating to surrogacy
+This clause provides for an offence with a maximum penalty of $10,000 for a person who publishes an advertisement, statement, notice or other material that seeks, or purports to seek, the agreement of a person to act as a surrogate mother for valuable consideration, or states, or implies, that a person is willing to act as a surrogate mother for valuable consideration.
+Part 6—Miscellaneous
+27—Provision of information etc for purposes of Births, Deaths and Marriages Registration Act 1996
+This clause provides that nothing in the measure affects the requirements in the Births, Deaths and Marriages Registration Act 1996 to have the birth of a child registered.
+28—Limitation of liability
+The clause provides that, except as specifically provided, no civil or criminal liability.
+29—Confidentiality
+The clause prevents the disclosure of information by a person obtained in the course of the administration of the proposed Act except to persons and in circumstances specified in the clause.
+30—Service
+This clause provides for the manner in which notices or other documents required to be given or served on a person under the measure are to be served on a person.
+31—Review of Act
+This clause provides that the Minister must cause a review of the operation of the proposed Act before the 6th anniversary of its commencement. the report is to be prepared and submitted to the Minister who must then lay a copy of the report before both Houses of Parliament.
+32—Regulations
+This clause allows the Governor to make regulations in respect of the proposed Act.
+Schedule 1—Related amendments and transitional provisions etc
+Part 1—Preliminary
+1—Amendment provisions
+This clause is formal.
+Part 2—Amendment of Assisted Reproductive Treatment Act 1988
+2—Amendment of section 3—Interpretation
+This clause makes a consequential amendment.
+3—Amendment of section 9—Conditions of registration
+This clause makes a consequential amendment.
+Part 3—Amendment of Births, Deaths and Marriages Registration Act 1996
+4—Amendment of section 4—Interpretation
+This clause makes consequential amendments.
+5—Amendment of section 22A—Surrogacy orders
+This clause makes consequential amendments.
+6—Amendment of section 49A—Saving provision—surrogacy arrangements
+This clause makes a technical amendment.
+Part 4—Amendment of Family Relationships Act 1975
+7—Amendment of section 10—Saving provision
+This clause makes a technical amendment.
+8—Amendment of section 10EA—Court order relating to paternity
+This clause makes a consequential amendment.
+9—Repeal of Part 2B
+The provisions in Part 2B of the Act are repealed as they are now to be contained in the proposed Act.
+Part 5—Transitional and saving provisions etc
+10—Continuation of recognised surrogacy agreements under Family Relationships Act 1975 as lawful surrogacy agreements
+This clause makes transitional and saving provisions consequential on the repeal of Part 2B of the Family Relationships Act 1975 and the enactment of this measure.
+Debate adjourned on motion of Dr Close.</t>
+  </si>
+  <si>
+    <t>The Hon. J.E. HANSON (16:33): Today I would like to reiterate the Labor Party's strong support for this legislation and, more broadly, to recognise and support the vital work our CFS and SES volunteers do. We are incredibly privileged in our state to be served by such an incredible group of dedicated volunteers, and it is well past time that their service and dedication is recognised in parliament and in legislation.
+The CFS and SES volunteer charters were originally launched during the Rann government in 2008, and since then they are reviewed and renewed every four years. The charters represented a commitment by the then government, CFS, SES and SAFECOM to consult with the volunteer associations and CFS and SES volunteers about all matters that might affect them. It is in that spirit that this bill seeks to enshrine those charters in law.
+This bill has been introduced previously in the other house. It was introduced by Duncan McFetridge, the then member for Morphett, in 2012 and in 2015. In the Legislative Council, it was introduced by the Hon. Robert Brokenshire in 2015, who is now back with his cows. However, when it passed the Legislative Council, it never made it to a vote in the other place.
+While the bill had broad support both in and outside of parliament, our volunteers have been left to wait for this simple reform to come to pass. They have been waiting for far too long now, particularly given the fact that Labor, the Liberals and the Greens have all previously voiced their sincere support for this reform. It is high time that this bill passed. In the words of the SES Volunteers' Association, I quote:
+The volunteer charter being delayed is an insult to our volunteers and has had many of them question whether the majority of members of parliament really understand the roles and commitment forthcoming to our state, the thousands of hours freely given to support the community, not even mentioning the millions of dollars donated through these hours.
+It is a really small reform. Putting into legislation that which already exists through regulation and in the charter is a really small reform, but it means the world to our CFS and SES volunteers to see their work recognised and to have firm commitment from this and future parliaments to consulting them and working constructively with them on matters that affect them.
+It has been over a year since this bill was introduced to this parliament. During that time, the minister then tried to incorporate its intent into his own bill following an unsuccessful select committee process and report—who would think that would happen? That a piece of legislation continues to languish in the other place with no sign of progress anytime soon is not encouraging. I am therefore pleased to see this bill and this issue being progressed here in the upper house instead, so that CFS and SES volunteers can finally have the certainty they have been after for so long.
+The volunteer associations are becoming increasingly frustrated with the inaction and the incompetence of the minister and, to some extent, the Marshall government and their inability to pass what is a very simple piece of legislation supported by the overwhelming majority of members. The volunteer charters are in recognition and commitment to SES and CFS volunteers who are at the coalface and understand their communities and their needs. Hence, their voices need to be recognised here.
+The Labor Party has always highly valued the positive contribution of the CFS and the SES Volunteers' Association to the emergency services sector as well as the strong advocacy they provide on behalf of all CFS and SES volunteers. As such, we are pleased to support this bill and commend it to the chamber.
+The Hon. S.G. WADE (Minister for Health and Wellbeing) (16:38): I rise to speak on the honourable member's bill to amend the Fire and Emergency Services Act 2005 and I indicate that I speak on behalf of the government. The government will be supporting the bill. The bill provides legislative recognition to the Country Fire Service and the State Emergency Service volunteer charters.
+As the Hon. Tammy Franks mentioned in her contribution, this bill is not a new matter for this chamber. It has been long foreshadowed. The move to enshrine volunteer charters in legislation can be traced back as far as the 2013 Holloway review, a review which the former government failed to act on. Previous iterations of this legislation were introduced in this place, although not, I note, by the former Labor government.
+Despite bipartisan support in this place, previous bills lapsed before passing the House of Assembly. The provisions within the bill before us today are reflected in those which have been introduced on behalf of the government by the Minister for Police, Emergency Services and Correctional Services in another place. The government will be pleased to support the bill.
+The Hon. C. BONAROS (16:40): As much as I do not like to disappoint the Hon. Terry Stephens, I rise once again on behalf of SA-Best—
+The Hon. T.J. Stephens: Point of order, Mr President, she is always trying disappoint me.
+The Hon. C. BONAROS: —to speak in support of the Greens' Fire and Emergency Services (Volunteer Charters) Amendment Bill 2018. The bill has a long history in this place, and I acknowledge the tireless work of former parliamentary members in that regard. As has been alluded to already, back in 2012 the former member for Morphett, Duncan McFetridge, first brought the bill before the parliament. Then, in September 2017, former MLC Robert Brokenshire reintroduced the same bill. Unfortunately, the bill lapsed in the House of Assembly after passing in this chamber on 15 November of that year.
+It is disappointing that there were other higher priorities for the former parliament, in its dying days, rather than making a small but significant change to the Fire and Emergency Services Act 2005. On that note, I commend the Hon. Tammy Franks for continuing the legacy of the aforementioned parliamentary members by once again reintroducing the bill to this parliament as one of the first private members' bills of this parliament.
+The bill provides legislative recognition to the respective volunteer charters of the South Australian Country Fire Service and the South Australian State Emergency Service. In effect, it takes the volunteer charters for both the SA CFS and the SA SES out of regulations and places them into legislation, which, as we all know, cannot be disallowed.
+The respective charters were first signed in 2008 and were relaunched in 2013. The CFS and SES volunteer charters were developed to recognise the value of emergency services volunteers, and specifically reiterate the government and emergency services sector commitment to consulting and considering the views, needs and interests of CFS and SES volunteers. They also identify the key roles and responsibilities of the parties to the charters, including the requirement by government, the South Australian Fire and Emergency Services Commission and the volunteer associations, to recognise, value, respect and promote the contribution of volunteer officers and members to the wellbeing and safety of the community.
+The charters provide a framework for all parties to work in partnership with each other in the best interests of CFS and SES volunteers and the broader South Australian community. Victoria already recognises the volunteer charter in the Country Fire Authority Act 1958, so I think it is only fit that we no longer delay that for SA. The bill also inserts new section 58A into the act, which gives legislative recognition to the SA CFS Volunteer Charter. In addition, there is also the insertion of new section 107A, which similarly introduces parliamentary recognition under the SES Volunteer Charter in the form of legislation rather than regulations.
+I note that the issue has broad support across all sides of politics, with it forming a pre-election commitment by the Liberal Party at successive elections. Indeed, the government included the volunteer charters in its Fire and Emergency Services (Miscellaneous) Amendment Bill 2018. That bill, as I understand it, was more extensive in scope. As a consequence of some of its more contentious aspects, particularly clause 23, it was referred to a select committee for inquiry and report. The report on the bill was, as we know, tabled on 4 April 2019, with the committee making a number of recommendations, particularly regarding further consultation.
+What is not controversial in the government bill is the volunteer charters. However, the government bill languishes to this day, and that is simply unacceptable. The volunteer charters should not, I believe, have been included in the miscellaneous amendment bill, and that delay is nothing short of an insult to CFS and SES volunteers, who I think we all agree deserve much better.
+If the government truly appreciates the unique and irreplaceable role played by the CFS and SES volunteer organisations, it would see the passage of this bill through both houses expeditiously, and it would also see the enactment of this bill as a matter of urgency. There are over 14,000 CFS volunteers and around 1,700 SES volunteers who put their lives at risk with every bushfire, every road crash, every storm and every lightning strike. They witness the unimaginable: the horrors of death and the horrors of destruction.
+During the 2018-19 fire season, CFS volunteers donated close to 500,000 hours of their own time to serve and protect South Australians. In dollar value that equates to more than $21 million, and we cannot underestimate the value of that unpaid contribution to this state. In a typical year, SES volunteers respond to around 10,000 calls for assistance from the South Australian community at any time of the day or night. Some of the busier Adelaide metro units respond to hundreds of call-outs each year.
+The SES is primarily responsible for responding to extreme weather, including storms, extreme heat and flooding events, and they also respond to road crash, marine, swift water, vertical and confined space rescues. They assist SAPOL in land search operations and traffic management and play an important support role to the CFS during major bushfires. 
+On behalf of SA-Best, I thank all the CFS and SES volunteers for their dedication in protecting the communities they serve. On behalf of SA-Best, we understand the commitment each volunteer makes in terms of these undertakings, the risk-prone work and the thousands of hours they give freely to support all South Australians.
+The bill and its predecessors are a culmination of a dedicated and long-held campaign by SA's CFS and SES volunteers. Their tireless work to have the CFS and SES charters enshrined in legislation arose from a fundamental concern of volunteers and their respective associations that existing consultation processes were inadequate in providing them with the confidence that their views would be listened to and given the gravitas they deserve.
+For those reasons, again on behalf of SA-Best, I commend them for persevering with their efforts and stand with them in wanting to see this legislative change to enshrine their respective charters in legislation once and for all. For the reasons outlined, I commend again the work of the Hon. Tammy Franks in that respect and indicate SA-Best's full support for the bill.
+The Hon. T.A. FRANKS (16:48): I would like to thank those speakers who have made a contribution today: the Hon. Connie Bonaros, the Hon. Stephen Wade and the Hon. Justin Hanson, and thank them for their support for this bill which, while small in its make-up, will be a very important bill for those volunteers. Indeed, it is a sign of respect for those who protect us, who put their lives on the line not as part of their career but in their volunteer hours. When they could be spending that time with family and friends or in recreation, they are out there, on the front line, defending us and our state, people and property.
+This has been a long time in the making. I acknowledge the previous work of the Hon. Robert Brokenshire and the former member for Morphett Duncan McFetridge. He was delighted to hear that this was finally going to a vote, when I spoke to him in the last few days. While I as a Greens member of this parliament quite often had very little in common with the Hon. Robert Brokenshire and sometimes with the former member for Morphett, on this, on support for volunteers in our emergency and fire services, we were always united, so I absolutely commend the work of both former members.
+The volunteer associations of the CFS and the SES are disappointed that it has taken so long to get to this point. This was a commitment made by all sides of politics in the previous parliament that passed this upper house unanimously but languished in the lower house without ever reaching a vote, that was an election promise from both sides, that a year ago I tabled thinking that the government would respond to with more urgency than they have. Indeed, if our emergency and fire volunteers took as long to turn up, we would be in a real spot of bother.
+However, I look forward to its speedy passage in the other place and the sponsorship of the member for Mount Gambier, Troy Bell, to ensure that this bill is finally made law and that we do indeed respect those who protect us.
+Bill read a second time.
+Committee Stage
+Bill taken through committee without amendment.
+Third Reading
+The Hon. T.A. FRANKS (16:53): I move:
+That this bill be now read a third time.
+Bill read a third time and passed.</t>
+  </si>
+  <si>
+    <t>The Hon. V.A. CHAPMAN (Bragg—Deputy Premier, Attorney-General) (10:39): I move:
+That this bill be now read a second time.
+I rise to speak on the Statutes Amendment (Decriminalisation of Sex Work) Bill 2018 and it is with much pride that I do so. I had wondered, given the history of this matter, whether we would ever come to this day, but I am proud to say that we have. The outline of the proposed legislation, which has had scrutiny through its introduction and passage in the other place, has been a valuable addition.
+May I outline first that the Statutes Amendment (Decriminalisation of Sex Work) Bill seeks to progress reform to remove offences relating to prostitution and the keeping of brothels from our criminal law, both the Criminal Law Consolidation Act and the Summary Offences Act. Furthermore, the bill ensures that current and former sex workers cannot be discriminated against under the Equal Opportunity Act and that they are covered through return to work provisions. Finally, the bill brings offences relating to prostitution, brothel keeping and street soliciting under the spent convictions regime, allowing prescribed sex work offences to be spent convictions. I will turn to each of these key components shortly.
+The bill I speak of today is nearly identical to the bill proposed by the Hon. Michelle Lensink MLC, introduced into this parliament in 2015, and that of Steph Key, MP of the time, introduced in 2013. The 2015 bill was subsequently the subject of a select committee report published on 30 May 2017. Although it was passed without amendment by the Legislative Council on 5 July 2017, that bill did not ultimately pass the House of Assembly prior to the prorogation of parliament.
+The bill before us today reflects the lengthy work of that committee and those members on it and takes into account amendments provided in the Legislative Council only weeks ago. I believe that these amendments work to strengthen the bill for our sex workers and brothel keepers but will also deal with some community concern around advertising and police powers.
+We are joined on this day by an historic group of people in the chamber, many of whom have paved the way for the full decriminalisation model to be progressed in our parliament and the basis upon which we are able to debate this today. Specifically, I would like to thank attendees from Zonta, the YWCA, the Sex Industry Network, SHINE SA, the Working Women's Centre, Business and Professional Women, and the Health Services Union.
+I would also like to thank the Hon. Tammy Franks MLC, the Hon. Michelle Lensink MLC, Duncan McFetridge, former member of this parliament, and my colleague the member for Reynell, who joins me today to second this bill. I also wish to thank the Hon. Steph Key and the Hon. Diana Laidlaw, who cannot join us today but who have been with us every step of the way in working towards a full decriminalisation model.
+As a firm believer in this cause, I see decriminalisation as the only model that will comprehensively afford sex workers and women their fundamental rights and protections. By decriminalising sex work, we can provide the predominantly female and often highly vulnerable cohort the opportunity to be afforded basic health care, report instances of abuse to the police, seek work opportunities and contribute to society without the overarching stigma of their choice of work.
+The sale of sex has existed since time immemorial and will continue to exist with or without the passage of this bill. However, the bill can improve the health and safety conditions of workers and reduce crime rates, which is the experience of other jurisdictions that have implemented decriminalisation. I refer particularly to New South Wales and New Zealand, which have decriminalised sex work in 1979 and 2003 respectively. This bill, at its heart, is about choice: the choice to work in whichever industry you like, the choice to disclose details of actions to the police without the fear of prosecution and the choice to cease working in the industry should you choose to do so.
+I will now move to key components of this bill. Under the bill, at clauses 9 to 19 inclusive, the protections of part 5B of the Equal Opportunity Act 1984 are extended to a former or current sex worker, which is to be defined as a 'person who provides sexual services on a commercial basis', and their relatives or associates.
+The amendments will have the effect of treating discrimination on the grounds of being or having been a sex worker in the same way that part 5B of the Equal Opportunity Act currently treats discrimination on the grounds of marital or domestic partnership status, the identity of a spouse or domestic partner, pregnancy, association with a child, caring responsibilities and religious appearance or dress. Generally speaking, it will be unlawful to discriminate against a former or current sex worker and their relatives or associates by treating them unfavourably in employment and education or in relation to land, goods, services and accommodation.
+Under section 6 of the Equal Opportunity Act, a person—that is, the discriminator—treats another unfavourably on the basis of a particular attribute or circumstance if the discriminator treats that other person less favourably than in identical or similar circumstances in which the discriminator treats, or would treat, a person who does not have that attribute or is not affected by that circumstance. The equal opportunity commissioner has advised that the amendments simply add a new ground to the act. The commissioner has no concerns about this, noting that exemptions can be applied for.
+Clause 20 of the bill allows for prescribed sex work offences to be spent convictions. Under this clause, convictions will be taken to be spent if they were an offence against keeping of a bawdy house, section 270(1)(b) of the Criminal Law Consolidation Act; permitting premises to be frequented by prostitutes, section 21 of the Summary Offences Act; soliciting in a public place, section 25 of the Summary Offences Act; procurement for prostitution, section 25A of the Summary Offences Act; living on the earnings of prostitution, section 26 of the Summary Offences Act; the keeping and management of a brothel, part 6 of the Summary Offences Act; or a common law offence related to prostitution.
+The Spent Convictions Act 2009 sets out the law on when a conviction is not disclosed on your criminal record. A spent conviction is a conviction that, subject to exceptions, cannot be disclosed on a police check and is not required to be disclosed in response to questions about criminal history. Some exceptions to this rule include certain categories of employment, character tests and screening applications. Unless applying for particular types of work, a person who has spent convictions does not have to disclose them to prospective employers, and employers cannot refuse to employ someone on the basis of spent convictions.
+Regardless, spent convictions are disclosable in relation to working or volunteering with children, people with disability, vulnerable people or people in the aged-care sector. This includes working with children checks. In these circumstances, the screening unit operated by the Department of Human Services undertakes an examination and consideration as to whether a current or former sex worker poses a risk to children and thus whether a working with children check should be granted. This is done on a case-by-case basis. Additionally, people with sex work-related spent convictions are eligible to apply to a magistrate for an order that their spent conviction is not disclosable, even in relation to these exceptional types of work.
+Clause 23 of the bill inserts police powers to enter and search premises used for commercial sex services if there is reasonable cause to suspect an offence has recently been, or is about to be, committed or to secure evidence of an offence. Under section 32 of the Summary Offences Act, currently police have the power to enter and search premises that are reasonably suspected to be brothels. Retaining a right of entry in certain circumstances is important when decriminalising sex work; however, it should not overreach the decision of parliament to decriminalise brothels and sex work.
+As such, this clause ensures that there is adequate and appropriate police power to enter premises used for commercial sex services where there is reasonable cause to suspect that an offence has been recently committed or is about to be committed. This clause ensures a balance is met between entering premises in the investigation of a crime and simply entering premises with no reasonable cause. There must be a reasonable cause to suspect an offence is occurring.
+The Commissioner of Police has noted their opposition to a bill that gives police no power to enter premises where crimes such as child exploitation, child trafficking or otherwise are occurring. South Australia Police are provided effective measures to protect sex workers from illegal exploitation, to prevent the involvement of minors and to prevent organised crime entering the industry, without a broad right of entry power affecting potentially much more of our community.
+Clause 24 of the bill repeals offences relating to soliciting in a public place for the purposes of prostitution under section 25 of the Summary Offences Act, procuring a person for prostitution under section 25A, and living on the earnings of prostitution of another person under section 26. The retention of these offences in their current form displaces the criminalisation model and erodes the purpose of this reform.
+Despite this, I have seen a strong interest from both sides of the parliament to see an amendment limiting where soliciting can occur. On the face of it, suggestions like the creation of declared precincts are utterly inappropriate as a solution to the supposed perils of soliciting, as I imagine we would simply see precincts encompass entire suburbs.
+Looking at the New South Wales experience, the New South Wales Summary Offences Act provides that a person on a road shall not, near or within the view of a dwelling, school, church or hospital, solicit another person for the purpose of prostitution. This model covers both soliciting clients by prostitutes and soliciting prostitutes by clients. I consider that a model akin to this may be a worthy option to ensure broader community concerns are addressed and will be considering amendments to the same.
+Finally, I turn to regulation and licensing. I do not believe that licensing structures have a place in any debate around the decriminalisation of sex work. This view is shared by current licensed jurisdictions like New Zealand, New South Wales and Queensland, which, I have been advised, are progressing towards full decriminalisation. South Australia has the opportunity to learn from the mistakes of other jurisdictions and progress with a fully decriminalised model, yet one which enshrines advertising restrictions, protections for vulnerable persons, exit assistance and police powers.
+I am acutely aware that other models proposed by decriminalisation opponents are simply a mechanism to detract from true reform. Quite simply, sex workers oppose licensing models on the grounds that it compromises their safety for similar reasons to the existing laws and shows ignorance as to what the decriminalisation of sex work means.
+The bill has been sent to the Law Society of South Australia for its comment and I look forward to sharing that response with this place and working with the society on any amendments that would add to the decriminalisation of sex work in South Australia. On that note, I encourage all members on both sides of politics to take an opportunity to meet with the Sex Industry Network and other advocates to learn about what decriminalisation truly means to someone on the front line.
+I urge members to hear about the way sex workers interact with members of our disabled community who might not otherwise have opportunities, hear about the stigma and derogatory behaviour that occurs on the streets and listen to the educated, bright and conscientious women leading this charge for reform. There have been significant miscommunications and mistruths about what this bill will and will not allow.
+In the coming weeks, I will be holding a comprehensive briefing with my colleague the member for Reynell, which I hope all members will attend. This is not a political issue. This is a basic question of fundamental rights and the rights for all to feel safe in the workplace. We need an open dialogue on this reform and I welcome all opinion and comment from my colleagues in this place and stakeholders in the wider community, but we must remain respectful during debate and outside commentary.
+I end with this: our parliament is left with two options. We either persevere with the status quo, effectively ignoring sex workers as the victims of crime and perpetuation of the stigma around this industry, or we progress with decriminalisation and see a stronger protection for workers and women. I implore all my colleagues on both sides of the house to consider this carefully and support the decriminalisation of sex work.
+Ms HILDYARD (Reynell) (10:54): I rise to second and speak in support of the Statutes Amendment (Decriminalisation of Sex Work) Bill. In doing so, I acknowledge the Attorney-General and thank her for her co-sponsorship of the bill and for her determination to work together to progress reform. I acknowledge the Hon. Tammy Franks and say thank you to her for bringing the bill to the other place and for her deep commitment to achieve decriminalisation.
+I heartily thank my friend the Hon. Irene Pnevmatikos for her wise contribution and unfailing support, support steeped in an understanding born from her lifetime of work to support and empower workers, of the deep link between decriminalisation and the positive health and wellbeing of sex workers. I also thank the Hon. Michelle Lensink for her leadership in progressing this decriminalisation of sex work, and I thank the many colleagues here and in the other place and those brave women who have prosecuted this argument before, Steph Key in particular, for their voice, for their tenacity and indeed for their endurance.
+I thank the incredible advocates and women's organisations here with us today, advocates and organisations that make all of us in this place feel stronger in our voices and in our actions and feel supported, which is a very special thing. To the YWCA, to the Working Women's Centre, Zonta, BPW, SHINE, Soroptimist International, the National Council of Women Australia, the South Australian Rainbow Advocacy Alliance, the women lawyers' group and the HSU, thank you for your deep conviction in advancing the interests of all women here in this state and beyond.
+To SIN, thank you for being with us today and for your advocacy, advocacy that I hope more workers will feel even more confident to seek out and openly connect with following a successful passage of this bill. This bill being at this point is testament to your exemplary work. Most importantly, I acknowledge the workers who are here with us today, workers who have shown enduring leadership, courage and tireless, relentless advocacy for what they know is right.
+I say to each of you that I know this fight has been a long one, filled with eternal hope and, to date, lined with disappointment as we have edged closer and closer towards decriminalisation. I say to you that I stand with you, I am here for you and, like all those I have just mentioned and members on both sides of this house, including the member for Bragg and the member for Cheltenham, who has been a strong advocate for change, I will keep fighting alongside you until this is won.
+History tells us that change and progress always happen when people relentlessly raise their voices together for as long as it takes to achieve that progress. Just like Catherine Helen Spence and her remarkable cohort of activist women, whose work 125 years ago meant that women here in South Australia could finally vote, we will not stop. Friends, we will get there, and it is indeed high time that we do.
+I had the opportunity to see some of the contributions in the upper house, to listen and to read the words of members. I was intrigued about the thread amongst those words about values, morality and what drives people to take a particular position. It was clear to me, as it so often is, that most people come to this place with a conviction born from experience, born from who and what has shaped them and born from their beliefs.
+I am confident that most who have contributed to date did so because they felt strongly about what the right or moral thing to do was for their own conscience and also for the rights and wellbeing of those whom this legislation will affect. It is the case, however, that we can reach different conclusions about how this law will or will not impact those rights and those people's wellbeing.
+I have talked with sex workers in this state for the past couple of decades, and I have heard them. I bring that deep listening to this place today, to this issue that we contemplate, and I also bring my own set of experiences that have shaped me, my own values, my own conscience and my moral compass. I put myself forward for election to this place because I passionately believe in fairness and equality, because I am driven to ensure that people are included and that they are able to live their lives with dignity and respect, free from stigma. I put myself forward because I care about every member of our local and broader community and believe that above all else they should be enabled to access their human rights, those core rights that mean they are treated with humanity.
+To me, that humane treatment of people, that equality of access to fundamental human rights, is all about morality. It is from my own early experiences, that I developed my burning and relentless passion for fairness. It is from those experiences, and with the guidance of my very strong and often very loud mum, that I learned to speak up for myself when things were not fair and then to speak up for others. But it is through organising workers and other community members to have a strong voice on the issues that they care about, that drive them and that impact their lives that I learnt that the most important thing we do as leaders is not just to find our own voice on our own rights but always, always to empower the voice of others on their rights.
+I am driven to do this with and for all, and for a range of reasons I have particularly worked with women to engender their leadership, their voice, their power, because women are still not equal in terms of how they are empowered to participate in community life, in work, in politics or in our economy. It remains that women are more likely to experience violence in their lifetime, and this issue we contemplate today is absolutely about power. It is about empowering women and other people, of course, to advance their rights, to ensure they can access protection, support, advocacy and health services.
+I know there has been much dialogue about how we empower women when we are talking about them engaging in transactions to provide sexual services. What we do know is that all people who are engaged in sex work in a criminalised environment are marginalised, deal with stigma and experience discrimination. This is so because of the fact that they do their work in a criminalised environment, and the manifestation of that discrimination is an inability to access workplace protections, outreach support, advocacy and health services, and it also has an impact on how they are able to negotiate with and report to police.
+What has also shaped me from an early age is my faith. It continues to do so. My Christian Catholic faith is fundamentally entwined with my unshakeable and deeply held belief that it is incumbent on each of us to love people, to offer kindness to people, to include, to accept people and to do what we can to ensure their place in our community and to ensure that their voice is heard. It is not my place, nor the place of anyone else here, to carve roles for ourselves as judges and, by virtue of that tenet, as saviours, but it is absolutely our place to make sure that with love, kindness and determination we do what we can to ensure that all people have access to their fundamental human rights. That is the right and moral thing to do.
+It is that desire to include people to make sure that their voice is empowered to access their rights, the dignity and the respect they need, that has meant that I have supported this decriminalisation cause for more than two decades. It is also, of course, my conversations with sex workers over those many years about what work is like without basic industrial rights, without access to health and safety protections, to safe reporting mechanisms, to safe access to advocacy groups and to health care without stigma that bring me to my very firm view that I share today—that every worker, every person, should be able to access the rights that we have created, the rights enshrined in laws that we progress over time as our community demands.
+We as leaders must be here for all South Australians, and from those conversations, from everything that I have read and that I have heard criminalising this work through our existing law and making many workers—the majority of whom are women—unable to access the rights in other legislation that the majority of our community do access, mean that we are not here for these workers. In fact, through this parliament's multiple failures to pass this legislation, we have failed them and we have failed our community.
+We know that our current law lets people down; we need to change it. Should we decriminalise sex work, workers will have the opportunity to access the rights and protections that are afforded through work health and safety legislation, through the Fair Work Act and potentially through other industrial instruments—basic safety nets that all workers should have the right to access. I know that some questions have been raised in the other place by the Hon. Rob Lucas about how this will work, and I answer some of those now.
+Like other workers, to access, for instance, the provisions of the Return to Work Act, a worker will need to show that they are indeed a worker as opposed to an independent contractor, and they will need to demonstrate that their particular work injury has arisen as a consequence of employment. That is clearly stipulated in section 7 of the act, which sets out that compensability for a work injury requires a connection with employment and that the injury arose as a consequence of that employment. Section 9 identifies the evidentiary provisions required to establish compensability. There is, of course, longstanding case law on this issue.
+The Hon. D.C. VAN HOLST PELLEKAAN: Mr Speaker, can I suggest that you allow the member some additional time to finish her speech.
+The SPEAKER: Is the member nearly done?
+Ms HILDYARD: Just about three minutes, I think.
+Leave granted.
+The SPEAKER: Member for Reynell, three minutes.
+Ms HILDYARD: Additionally, the act in section 4 sets out what constitutes a contract of service. It can include a verbal or written contract, an award or understanding. In relation to any claim for compensation, evidence is required to establish the employment relationship. Again, there is much case law in relation to how that employment relationship is established. In terms of the Hon. Rob Lucas's questions about establishing average weekly earnings in relation to a claim, sections 5 and 9 of the regulations and section 5 of the act identify the key principles and concepts that must be considered in establishing the worker's average weekly earnings.
+Having for many years represented workers on issues around independent contracting versus employment, I could not say that the system is perfect nor that it provides the best possible outcomes every single time. That is not a reason to exclude one particular group of workers from accessing rights enshrined in legislation that all other workers are afforded. It is also an issue that we can assess post the passing of this bill. Wherever there are industries where there is a prevalence of workers being inappropriately deemed as independent contractors, resulting in a lack of access to industrial rights, it is important that we look at the industry to see how we can address that particular situation, how we can ensure the right environment is in place for them as workers.
+The bill, as the Attorney-General has pointed out, does rightly provide protection through the Equal Opportunity Act, protection that means workers will have an avenue for redress should they experience discrimination as a result of being or having been a sex worker. It also deals with the spent conviction issues. There are many other issues which we can of course also assess and for which I know there is a commitment to exploring the best possible outcomes. I can indicate to this house that following the introduction today we will be conducting a comprehensive briefing for all members. There is a commitment from both the Attorney and myself to working through the issues and questions that people rightly have, to providing facts, to dispelling myths and to making sure you have access to the people you want to talk with as you contemplate your position.
+In closing, I deeply believe it is time for us to move forward. It is no longer okay for a group of South Australian workers to be stigmatised, to be marginalised through fundamental unequal access to rights and protections. It is time for sex workers to be safely heard, to safely access health care, to seek out advocates and to report incidents without fear. It is time for sex workers to have avenues to safely pursue those who exploit them or perpetrate violence against them. It is time for us as a parliament to be honest about the fact that sex work is work and, just as we would in relation to any other job, it is time for us to provide access to the protections, the rights, the dignity and the respect that workers in the industry deserve.
+When this industry is decriminalised, we will better understand it. We will be able to work with sex workers to make sure that any limitations in rights and protections are addressed, to make sure that their voices are heard. Is that not one of the reasons we are here: to ensure people's voices are heard, to represent, to speak up for, and to progress rights for those most marginalised? I commend this bill to the house.
+Debate adjourned on motion of Mr Pederick.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr COWDREY (Colton) (11:31): I move:
+That this house—
+(a) welcomes the federal Liberal government's commitment to the $90 billion shipbuilding program, which will secure the future of South Australia's defence industry for decades;
+(b) notes the significant work being undertaken by the South Australian government to ensure that South Australians can reap the maximum benefit of the shipbuilding program; and
+(c) notes the significant negative impacts on the current workforce as a result of the former federal Labor government's failure to progress any future shipbuilding contracts during its last term in office.
+Together, we stand on the brink of a never before seen flow of work into South Australia. The only reason for this work coming is that the federal Liberal government has committed $90 billion of taxpayers' money over the coming decade to modernise and strengthen Australia's naval forces, which will build a strong and sustainable sovereign Australian shipbuilding industry.
+'Sustainable' is the key word that those opposite seem to have a tough time coming to grips with. Let us never forget that, during the Rudd-Gillard-Rudd federal Labor quagmire, zero—yes, zero, nought—vessels were commissioned, causing a massive hiatus in the work done at Osborne. Too often, those opposite conveniently forget that fact. In contrast, 54 separate vessels have been commissioned by the federal Liberal government. They will create a huge amount of work coming right here to South Australia, and particularly in the western suburbs of Adelaide, in which the electorate of Colton sits. This work will be here for generations to come and that is very good news for the people of our great state.
+Currently, two offshore patrol vessels are being built by ASC Shipbuilding, with production directly employing up to 400 workers at Osborne and sustaining 600 indirect jobs. In addition, the redevelopment of the Osborne South Shipyard, a colossal structure where the Hunter class frigates will be assembled, is underway. In parallel, the Naval Shipbuilding College is also well underway. This is just the beginning. Naval shipbuilding is set to deliver an unparalleled economic benefit to our state. Around 5,200 direct jobs will be created through naval shipbuilding activities in South Australia plus more in the supply chain, the training sector, the education sector and other associated opportunities.
+The next chapter in this book of good news is the landmark contract to build 12 Attack class submarines here in South Australia, a $50 billion project. The Attack class submarines project is the largest defence procurement in our nation's history, which is something we should all be very proud of. The project will set a number of national firsts in scale, in size, in complexity and in duration.
+Earlier this month, the Premier attended the Strategic Partnering Agreement signing in Canberra, where the agreement between the Australian government and the Naval Group was formalised. To date, work on the submarines had taken place under the design and mobilisation contract. The signing is a key step in the procurement process, with the agreement representing the contractual basis to the Attack class submarines project. The $35 billion Hunter class—
+Mr Malinauskas: What is the local content requirement?
+The SPEAKER: The Leader of the Opposition is called to order for interjecting something about local content.
+Mr COWDREY: —frigate program, which will deliver nine antisubmarine frigates to the Royal Australian Navy, will create and sustain 1,500 direct jobs. In addition, 600 jobs are needed for the redevelopment of the Osborne South Shipyard and opportunities through that supply chain. These opportunities include many South Australian-based businesses—for instance, structural steel for the mammoth shipyard has been sourced by South Australian-based steelmaker, Liberty OneSteel in Whyalla. The opportunities around naval shipbuilding are not just in Osborne, Port Adelaide or more broadly in the western suburbs of Adelaide, or at Lot Fourteen. No, the opportunities that a strong and sustainable naval shipbuilding program provides will have positive impacts and flow-ons throughout our regions and our state.
+The Defence Landing Pad, to be located in Adelaide's new innovation neighbourhood at Lot Fourteen, will provide a home for global companies to develop their Australian business strategies and plan local operations. It will add to our already thriving prime and associated contractor environment a new one-stop shop supporting international defence companies to establish in South Australia that will drive defence industry investment. The Defence Landing Pad will enable international businesses to build relationships with South Australian businesses and create opportunities for our supply chain collaboration.
+This is just one example of what the Marshall Liberal government is focused on: ensuring that we as a state make the most of the significant opportunity and investment that the federal government has made in naval shipbuilding here in South Australia. It is our obligation and our responsibility to ensure that we build capability, that we as a state make ourselves known for these skills and these industries and in the future seek further opportunities so that the impact of these investments lasts far beyond the already committed works.
+The Minister for Industry and Skills tells us, sometimes ad nauseam, about the 20,800 new apprenticeships and traineeships, but the program is incredibly important. It is important because we need to work hard and make sure that we have the requisite skills in place to deliver on these projects. It is an incredible opportunity for our young South Australians, our next generation. They have an opportunity that those before them did not.
+The Marshall Liberal government is committed to maximising the local benefits of this huge investment into our state and, as I said, this includes ensuring that we have the skilled workforce needed to deliver this project. Investing in training equipment like welding simulators and providing funding for additional work-based apprenticeships will help us create the skilled workforce that is required to fully capitalise on the naval shipbuilding program.
+As I mentioned, the Naval Shipbuilding College, a fantastic new facility, is also underway and will play an important part in preparing our state for the jobs of the future and the skills that we need for our future. In addition to new apprenticeships and new traineeships, the Marshall Liberal government is also introducing the following measures to further develop South Australia's skilled workforce. We are working with industry to strengthen South Australia's VET system, including giving industry a stronger voice through the re-establishment of industry skills councils.
+We are reforming the subsidised training list so that it is guided by industry and opening up funding contestability. We are establishing a new technical college in Adelaide's western suburbs, with a focus on defence and naval shipbuilding. The opportunities naval shipbuilding presents are not limited to advanced manufacturing, to engineering, to project management or to the trade sectors. 
+Just yesterday it was reported that the education and research sector is also already seeing benefits. It was reported that Adelaide University, Flinders University and the University of South Australia have signed an agreement with French company Naval Group, working on the subs, and France's National Centre for Scientific Research to fund an international research laboratory in Adelaide. The research lab will work on artificial intelligence, autonomous systems and ergonomics, also known as human factors. It is reported that Lot Fourteen, on the old Royal Adelaide Hospital site in the Adelaide CBD, is likely to play host to the lab, with hubs expected to be placed at each of the universities.
+All vice-chancellors of the three universities are supporting this announcement. The Vice-Chancellor of the University of Adelaide, Professor Peter Rathjen, said that he welcomed further collaboration with CNRS, Naval Group and the defence industry. The Vice-Chancellor of Flinders University, Professor Colin Stirling, said that Adelaide was an ideal location for the laboratory. The Vice-Chancellor of University of South Australia, Professor David Lloyd, also welcomed the collaboration. Quite frankly, this level of collaboration between our universities is unheard of. The scale and breadth demonstrate the opportunities associated with naval shipbuilding and the commitment that the federal Liberal government has made.
+Sadly, due to the federal Labor inaction I mentioned earlier, the Australian government has had to put in place, and backdate to 1 July 2018, the ASC Shipbuilding Structural Adjustment Program to support workers who, unfortunately, have been made redundant. Through this program, workers and their partners from ASC Shipbuilding or an affected supply chain business are supported through immediate access to intensive employment opportunities through Jobactive employment providers, including job search, résumé preparation, preparation for interviews, retaining, self-help facilities, skills assessments and career advice workshops. In addition, they have been provided with assistance by way of a $2,000 employment fund to assist workers to retain and obtain licences and tickets, as well as relocation assistance, if it is required.
+As a member of this place, as a Liberal, as a South Australian and as a proud member of the western suburbs, I am incredibly proud of the commitment that the federal government has made by way of naval shipbuilding here in South Australia. I am incredibly proud to be part of the Marshall Liberal government, which is ensuring that we make the most of these opportunities for our local community and for our state.
+Mr MALINAUSKAS (Croydon—Leader of the Opposition) (11:42): I move to amend the motion, as follows:
+Delete paragraphs (a), (b) and (c) and substitute the following:
+(a) welcomes the 2016 defence white paper and the 2017 Naval Shipbuilding Plan and its commitment to developing a national naval shipbuilding capability;
+(b) calls on the federal government to secure a guaranteed level of Australian content in current and future shipbuilding programs to ensure the development of a national naval shipbuilding capability; and
+(c) calls for an independent naval shipbuilding authority to oversee the level of Australian content in future shipbuilding programs.
+Over the years, all of us in this chamber have heard ad nauseam the sort of speech just given by the member for Colton. More recently, the South Australian public has become accustomed to both sides of politics trying to claim credit for the fact that we now have an extraordinary opportunity coming our way in the form of the submarine program, with the Future Submarines being built here in South Australia. Truth be told, both sides of politics have had a hand in this exercise. We know that, if it were not for the ferocious campaigning and fighting for our state, the Future Submarines build was going to Japan. That is now a commonly accepted fact.
+Equally, we also know that on the back of that pressure coming from state and federal Labor, it was ultimately a federal conservative government that changed their tune on sending the work to Japan and instead opted for a sovereign capability here in Australia, with the Future Submarines being built in Australia by the Naval Group.
+So let's dispense with the tired old arguments around who can claim credit for what in regard to future sub builds. Instead, let's just focus on what is actually going to happen for our state in the future because I think we are all very cognisant of the fact that this is now an extraordinary opportunity. This is not just a once in one generation opportunity but a once in multiple generations opportunity. This is not likely to be something that we are going to see come to our state again in the future. We must make sure that we do everything that is humanly possible to maximise the opportunity for this state and all the chances for jobs that are coming our way.
+What we have seen over the last fortnight is a dropping of the ball when it comes to ensuring the delivery of jobs for our economy, because what we know is there is a legitimate contest. It will not surprise people that in France they view the awarding of the submarines contract to Naval as an extraordinary opportunity for the French economy. The Naval Group is celebrating this as a boon for French jobs. French politicians are celebrating this as a winning of the industrial Olympics for France. 
+So quite understandably, quite rationally, quite pragmatically, the French will do everything they can to maximise the opportunity of this $50 billion Australian investment delivering for French jobs. It is equally important that we as a nation and that we as a state acknowledge that legitimate competition and do everything within our power to ensure that jobs will be delivered here in South Australia.
+As the member for Colton referred to in his remarks a bit over a fortnight ago or thereabouts, a very important contract signing occurred interstate between the Commonwealth of Australia and the Naval Group: the strategic partnership agreement. The federal Minister for Defence, minister Pyne, was present, obviously, for the signing. Indeed, the Premier flew over for this photo opportunity. This event seemed to fly below the radar. One would have thought that the signing of the single biggest strategic partnership agreement for the largest procurement that our nation has ever entered into would have received a little more fanfare than just a singular quiet photo opportunity.
+Quite a few of us in state and federal Labor were taken a little aback that there was not much fanfare associated with such a significant event, and now we are starting to learn why. As information has started to filter out about this strategic partnership agreement, we have learned that there are some very real and legitimate concerns about whether or not that agreement is going to deliver the level of local procurement that all of us in South Australia want to see and whether or not it is going to deliver the real jobs that we have been promised. Let's just have a quick look at the historical context.
+With the Collins class submarine, the current class built here in South Australia on the back of advocacy from state Labor and delivered ultimately by federal Labor—but put that aside—we know that approximately 70 per cent of all the work that has occurred on the Collins class submarine has been done with local content. Look at another program: the Anzac class of frigates. We know that they have delivered about 80 per cent of local content for Australia.
+So where are we at with the submarines—the future build—the largest ever capital project that the Commonwealth of Australia has ever entered into since Federation? What is the local procurement requirement in the strategic partnership agreement? What is the minimum local content standard? Well, we have learned that there is none—none. There is no local content requirement in the strategic partnership agreement from the information that we have garnered through forensic inquiries made in the Senate estimates process.
+If that does not have everybody alarmed about how many jobs are actually going to come our way, then I am not too sure what will. Yes, it is true that there are clearly going to be jobs from the submarine build in South Australia, but are we maximising this opportunity? Are we doing everything we can? Where was the Premier's advocacy, where was this government's advocacy, in trying to secure a local content requirement?
+We have heard nothing. We have heard nothing but complete silence, and that is borne out by the fact that there is no local content requirement within this agreement. There are plenty of people in local industry who are genuinely concerned about this, as well they should be. We know that if you are going to have a local content requirement in such a contract, it would exist in this one. That is what the pundits tell us. That is what one would reasonably expect—that an agreement of such importance would contain some reference to local content, yet we know there is none.
+Of course, this comes on the back of some pretty large promises that have been made by the conservative side of politics when it comes to local content. We know that a 90 per cent number was thrown around that people were trying to have an association with. We know that minister Pyne himself referred to 60 per cent plus local content. In December last year, minister Pyne said that these jobs would be delivered through an assured level of local content. He told journalists, 'This will be a local build. A local build is defined as being around 60 per cent plus.'
+So we expect this to be a local build, yet we find out what the Strategic Partnering Agreement actually says: nothing. It is utterly delusional for anyone in this place, particularly people who are responsible from the party or the government, to suggest that they can now guarantee that 60 per cent figure when the very agreement that underpins this contract has no reference to local content. What guarantees and assurances can the Premier of this state or the member for Colton give the people of South Australia that we are doing everything we can to maximise this opportunity? None, it turns out—none.
+It is starting to demonstrate a bit of a pattern in the way this government behaves when dealing with the Commonwealth of Australia. It turns out that the modus operandi of this conservative Liberal government is to take their orders from their conservative Liberal mates. We have seen it on the Murray, the way they sold us out of our 450 gigalitres of upwater, and now we have seen it on the most important opportunity that this state has ever had in its history: being able to build the single largest procurement engagement exercise that has ever occurred in the history of Federation. Let it be known that on this side of the chamber we will do everything we can to fight for South Australian jobs, not capitulate and kowtow to their masters in Canberra.
+Mr BROWN: Mr Deputy Speaker, I draw your attention to the state of the house.
+A quorum having been formed:
+Mr McBRIDE (MacKillop) (11:53): I rise to speak in support of the motion put by the member for Colton:
+That this house—
+(a) welcomes the federal Liberal government's commitment to the $90 billion shipbuilding program, which will secure the future of South Australia's defence industry for decades;
+(b) notes the significant work being undertaken by the South Australian government to ensure that South Australians can reap the maximum benefit of the shipbuilding program; and
+(c) notes the significant negative impacts on the current workforce as a result of the former federal Labor government's failure to progress any future shipbuilding contracts during its last term in office.
+The $90 billion shipbuilding program committed to by the federal Liberal government has been a landmark decision which will reap benefits for South Australia for many years to come. The decision will modernise and strengthen Australia's naval forces and will underpin employment, build workforce capacity, investment, innovation and experience in shipbuilding in Australia. In particular for South Australian investment, it will yield significant economic benefits. The investment will create significant supply chain growth opportunities which are in addition to the more than 5,000 direct jobs that will be created through naval shipbuilding activities in South Australia.
+The funding will enable the build of 12 Attack class submarines, which I am told is the largest defence procurement initiative in Australia's history. The funding will enable a $35 billion Hunter class frigate program, which will deliver nine antisubmarine frigates to the Royal Australian Navy and will create and sustain 1,500 direct jobs. This will be in addition to the 600 jobs needed for the redevelopment of the Osborne South Shipyard and provide opportunities through the supply chain. The supply chain benefits will be substantial. The new Lot Fourteen innovation neighbourhood will provide a location which will attract global companies to develop their Australian business strategy and plan local operations.
+A new one-stop shop, supporting international defence companies to establish in South Australia, will drive defence industry investment. The Defence Landing Pad at Lot Fourteen will enable international businesses to build relationships with South Australian businesses and create opportunities for supply chain collaboration. The investment by the federal Liberal government will assist in bridging the unemployment vacuum that was created by the previous federal Labor government's lack of vision. Unfortunately, it dropped the ball regarding Australia's shipbuilding industry and its workers.
+We know that in Osborne today the last program is winding up. I can tell you that there are still employees there today being told that their jobs are about to finish. The contract is now winding down and their jobs no longer exist until this shipbuilding operation is back up to speed, back on the build, where it should have been four or five years ago. We know that there are some employees being re-engaged down there, but they are not the same ones who have been told their job no longer exists because they have come to the end of that contract.
+It shows that if this is going to be managed—and not to play politics with this and say that one side of politics is better than the other—it will require a united front on both sides of politics to recognise this as a big build for Australia. If we work together on the fact that it needs to happen in a methodical way that looks after the federal government's interests, the state government's interests and those of employees, contractors and builders alike, then it can be an absolutely wonderful opportunity for Australia.
+To summarise, we know the new patrol boats are just starting off. I believe there are going to be two built in Adelaide to start off with, of the perhaps 12 that Australia will build. It is a starting point. They are employing people who start off by doing the groundwork, what we call laying down the keel. They will be building the bulkheads. There are no electricians yet. They are not mechanics, they are not chippies, they are not electricians or technologists with technical expertise, because they are not required right now. Those areas of expertise are not needed.
+This is where the vacuum and the lack of cohesion from one build to the next needs to be absolutely methodical and straightforward so that all employees in this region can have a job from one week to the next, one month to the next and one year to the next. This is so we can create consistent work in a consistent workplace where people can live their lives, build houses and dreams and know that this work will continue for many years to come.
+The ASC Shipbuilding Structural Adjustment Program, announced by the Australian government, will support workers who have been made redundant, and it will be backdated to 1 July 2018, because of the lack of foresight by our federal Labor government. I am advised that workers and their partners from ASC Shipbuilding or an affected supply chain business are also eligible for this program. The program will offer a range of services for employees both before their positions are discontinued and after. The types of services offered will include career advice, skills assessment and labour market information to assist people to make decisions on their next steps.
+The service will also include intensive employment support through Jobactive employment providers, job search support and retraining. This program will include a $2,000 employment fund to assist workers to retain and obtain licences and tickets, as well as relocation assistance if required. The investment by the federal Liberal government and the efforts of the Marshall Liberal government in continuous naval shipbuilding will create thousands of jobs for decades to come. There will be a period of supported transition as our current shipbuilding workforce redeploys to new opportunities being created across our defence industry base. Two of the offshore patrol boats are currently being built by ASC, with production directly employing up to 400 workers at Osborne and 600 indirectly.
+This gives me a bit of an opportunity to address the comments made by the member for Croydon (the Leader of the Opposition), who talked about the Collins class submarines and the history of Australian shipbuilding, as we know it so far. I do not want to play politics, but I want to make sure that our Liberal government recognises that it actually does take effort to ensure this will be a good and profitable build and one that builds a product that we can be proud of for many years to come.
+I note that the six Collins class submarines that were started in 1990 and finished in 2003 were costed at $4 billion to start off but blew out to $5.1 billion—27 per cent; $5 billion to $4 billion is not much. This is a $90 billion build, and if we blow out that budget by 27 per cent, that is an extra $24 billion that this one overall contract will cost if we do not do it properly. It will blow out to $117 billion on the same basis as the Collins class submarines.
+The opposition leader is worried about local content. Belonging to the Liberal Party government, I too want as much local content and build in South Australia as possible, but not at any cost, not at any blowout for many, many years beyond what it is meant to be. Absolutely, these boats have to work. There were six Collins class submarines. They only ever had, at some stage, a 35 per cent workforce working on the submarines because they were such high maintenance dependent. They were costing a fortune to maintain and operate. It was not just the worker base but also the fact that the Collins class submarine had huge issues of maintenance and standard.
+One of the biggest pitfalls, they tell me, is that we changed our mind during the build. The defence system wanted this and then they wanted that, and then it did not fit and then it did not work, and they would not talk each other. Technological advances were always on the go. One of the things that I hope we do with this large contract is to make sure that this build is a good fit, works for Australia's purposes, does not blow out and is not at any cost. This is unlike the Labor Party on the other side, which says: 'Just employ people, just spend money, just get jobs.' No, not at any cost at all.
+From my own history, having trained as a boilermaker/welder through an apprenticeship program, I am really excited about the investment the Marshall Liberal government is making to build the capacity and capability of South Australians. The program is going to yield a great many benefits for trade industries and it will provide opportunities for trainees. The more than 20,000 new apprenticeships and trainees that will be created have been made possible through the federal government's Skilling Australians Fund. They will offer really great opportunities for people to upskill and reskill in order to take advantage of new employment opportunities like this shipbuilding program.
+These positions will be supported by the establishment of a new technical college in Adelaide's western suburbs, with a focus on defence, and a range of other measures, including the re-establishment of industry skills councils to give industry a strong voice and a pathway to work, with government to strengthen and influence the vocational education training system. I commend the motion to the house.
+The Hon. Z.L. BETTISON (Ramsay) (12:03): I rise to speak on the amended motion. One of my motivations for being in politics was employment. When I finished school and university, it was really difficult to get a job. I had fantastic mentors. My parents both worked. They had a business, and they supported post secondary education. My concern today is this issue because when I am out doorknocking people ask me, 'What are the jobs of the future? What will my children do? What will my grandchildren do?' We know that we have a fantastic opportunity in South Australia with this shipbuilding program. We all agree that this is a wonderful opportunity.
+There are discussions that there will be up to 25,000 jobs in South Australia, so imagine my disappointment and my surprise that there is absolutely no commitment to local content. How do we expect our parents and grandparents to encourage their children to train in the areas that are going to be needed for this shipbuilding program?
+I acknowledge the Skilling Australia program and I acknowledge the Naval Shipbuilding College, but what we need to do is make all South Australians aware of what the jobs are and the pathways to get those jobs. Whether it be an electrician, a mechanic, a welder, a fitter and turner, like my own father when he did his apprenticeship, or be skills in technology or design, we know that those jobs are going to be needed.
+What we do not know is if those 25,000 proposed jobs are ever actually going to happen, because what we hear is the politics being played out. When we hear people being told in November 2017 that we are going to create 25,000 jobs in South Australia, and in December 2018 being assured by minister Pyne that these jobs will be delivered through an assured level of local content, that this will be a local build, that is what our parents and grandparents hear. 'Fantastic! This is what we are going to encourage our children to do.'
+We know that science, technology, engineering and mathematics are going to be crucial in taking up these jobs. I am excited about it. This is something that we can share. We can be part of world's best practice of this amazing advanced manufacturing. We welcome it; this is fantastic. But when we hear that there is no guarantee of local content, how can we say this to our South Australians? How can we encourage them to train in this sector? This is the concern that I raise with this issue today.
+What I am very concerned about is our Premier not standing up for our state. Sure, he might have been there for the signing, but where is his commitment, where is our understanding of the state government supporting, encouraging and knowing how many of these jobs there will be? That is why I rise today to support the amended motion.
+Mr PATTERSON (Morphett) (12:07): I rise to welcome the federal Liberal government's commitment to the $90 billion shipbuilding program that is centred in this state and to speak in support of the member for Colton's motion. We know that as the program to build air warfare destroyers at the Osborne naval shipbuilding precinct comes to an end, the federal government is now centring its naval shipbuilding program in South Australia, with the construction of the first two offshore patrol vessels, followed by the Future Frigate program and the submarine program.
+This $90 billion commitment will modernise and strengthen Australia's naval forces. We know that ASC has built up considerable skills over the last 10 years on the air warfare destroyer program, and the highly skilled shipbuilders, in conjunction with this new naval shipbuilding program, can be the basis for building a strong, sustainable sovereign Australian shipbuilding industry. It will certainly define the future of advanced manufacturing in Australia and it is happening right here in South Australia.
+These first two offshore patrol vessels are going to be constructed in South Australia by ASC and will overcome the valley of death between the end of the air warfare destroyer program and the beginning of the Future Frigate program. Unfortunately, prior to the commitment of the construction of these first two offshore patrol vessels at Osborne, the gap saw the steady release of the workforce and hence the loss of valuable skilled workers prior to the commencement of the Future Frigates shipbuilding program.
+It was therefore welcome news when in November 2018 work began on the first of these offshore patrol vessels at Osborne, with the welding of the first two component blocks of steel that will form part of the first vessel. The new ships will be known as the Arafura class, with the first to enter service in 2022 to be called the HMAS Arafura.
+The ASC chief executive noted </t>
+  </si>
+  <si>
+    <t>Adjourned debate on second reading.
+(Continued from 16 May 2018.)
+The Hon. I. PNEVMATIKOS (16:54): Today I rise to speak on the Statutes Amendment (Decriminalisation of Sex Work) Bill (No. 2). This is a matter that has been debated many times in respect of how it should be governed. In fact, in the last 20 years there have been 12 bills introduced to decriminalise sex work and none of them has been successful. Why? Because it is a contentious issue, heavily cloaked in stigma. More oft than not, the moral values and personal beliefs of a few have drowned out the voices of the many and, in particular, those on the front line. Voices such as Scarlet Alliance, SIN, the World Health Organization and the workers themselves, who are willing to risk a great deal to be seen, heard and taken seriously.
+I agree that this is fundamentally a moral debate. I am certainly not referring to any perceived morality of sex work. I am referring to the morality we have as a society to ensure that every person is afforded the same fundamental rights and protections. This must be our moral imperative, first and foremost. We cannot allow personal ideologies to overshadow the issue at hand, workers' rights and the views of the general public on this issue.
+As recently as today, ABC Adelaide conducted a poll on whether sex work should be decriminalised. Out of over 5,300 votes, 93 per cent agree with decriminalisation, yet South Australia remains one of only three states in Australia where sex work remains criminalised. Our laws here are generally regarded as the most harsh and punitive. This must change because it is detrimental not only to sex workers' safety, health and wellbeing but also to the whole community. We need to end the marginalisation and discrimination. We cannot allow people in this state to continue to live without many of the legal and social protections afforded to the general population.
+We on this side of the divide, as the Labor Party, have strong and important connections with the labour movement. This bill should be supported, like any other bill, for the benefit of workers and their families. All the studies support the fact that, as long as sex work is criminalised, sex workers often have to choose between safety and legality. We would not condone this in any other industry and we cannot continue to condone this for the sex work industry. Decriminalising sex work will provide a protection to sex workers and ensure that their basic human and labour rights are upheld.
+As a society, we do not get to pick and choose whose human rights, working conditions or health and wellbeing we protect. These are fundamental universal rights and they must be afforded to everyone. It is no coincidence that organisations such as the World Health Organization and Human Rights Watch have all spoken out in favour of decriminalising sex work. In fact, for us to honour our commitments as a signatory to the UN Political Declaration on HIV and AIDS we need to enable decriminalisation.
+We know that criminalisation poses substantial obstacles in accessing HIV prevention, treatment and support. We have seen in New South Wales and New Zealand that decriminalisation has had a significant impact on reducing HIV and other STI transmissions. In fact, more so than any other regulatory models.
+There is no doubt that one of the biggest challenges in this debate is ignorance. Ignorance stems from relying on stereotypes and preconceived notions of sex work instead of factual information. In fact, it is ignorance that causes stigma. Sex workers, activists and experts alike agree that stigma is one of the greatest obstacles preventing sex workers from enjoying the same rights and access to support that the rest of us take for granted.
+Rather than seeing and understanding the complexities, members' perceptions in this place have in the past been clouded by their personal beliefs of what is shameful, sinful or evil. I have read through previous transcripts, transcripts that hide behind religious arguments based on ideas that sex work is deviant and a source of moral decay, and arguments and fears that the model will threaten the very foundations of marriage and our society as we know it.
+Let me just say that decriminalisation has occurred in other states and in New Zealand, and guess what? The sky did not fall. As put by a sex worker last Friday on the steps outside parliament, 'If you fear for your marriage, ask us if your husband or wife has been to see us. Criminalisation will not change the probability of infidelity.'
+Concern with the profession becoming a more popular choice for children is another common concern raised in this place. This is purely a manipulative argument to support discriminatory attitudes. Take, for example, Roxanna, who has been both a sex worker and a PhD student in the School of Psychology, Social Work and Social Policy. She provided me with a compelling thesis on sex work in the South Australian context. She would not fit the mould that many in this place would paint about sex workers.
+On the note of children, let me make it clear that when debating this matter I do so with the focus on adult workers in the industry: women, men and those who are transgender. In no way do I condone exploitation of children, nor does this bill create an avenue for that. I strongly believe that criminality creates an us and them mentality, resulting in systemic and tolerated discrimination that can affect a person's access to housing and accommodation, employment opportunities and justice.
+Stigma is socially isolating and shaming, and this makes sex workers vulnerable, because they are less likely to report violence or abuse or to seek help and support. Unfortunately, we will hear arguments in this place that through decriminalisation we will see more violence against women. This is a play on the stigma associated with the industry, and it also blatantly disregards the laws that are already independently in place to support violence against women. It is a facade to hide behind to protect religious and traditional morals. It is not a consideration of the contents of this bill.
+We will also hear arguments that decriminalisation does not support the feminist agenda, that sex work is perpetrated on women. As put by Elena Jeffreys of Scarlet Alliance:
+…sex work is feminist—being sexually active, putting a value on your sexual interactions, negotiating boundaries and making informed choices about your body.
+Some may even argue that decriminalisation will lead to trafficking. Again, this argument blatantly ignores federal laws already in place to tackle this issue. If the existing laws fall short in any way, then let us look at those laws and strengthen them. They are not arguments that have anything to do with this bill. As I said earlier, stigma is dangerous and creates secrecy where what we need is exactly the opposite: dialogue and greater understanding.
+Some in this place will argue for an alternative model which decriminalises the selling of sex but criminalises the client. I have given this model heavy consideration and, whilst on the outer layer it appears to be designed to protect women, there is empirical evidence that this model propels the idea that sex work is violent towards women and further marginalises women in the industry.
+A major survey analysing this model, Sex in Sweden, also highlights that the model creates an environment where sex workers need to be less visible. It successfully displaces street-based sex work by placing sex workers in a position where they experience further difficulties with the authorities and law enforcement, and have less negotiating power with their clients, specifically regarding safer sex practices.
+The bill currently before parliament will not only decriminalise sex work but will also prohibit discrimination against sex workers and ensure that sex workers can enjoy the same rights and protections as other workers. Importantly, it will ensure that when sex workers experience exploitation or violence in any way, including from clients, employees, the police or others, these crimes are dealt with promptly and justly, just like any other crime.
+Decriminalising sex work will allow us to better understand an industry and its workers and ensure that safeguards and regulations are in place to protect all. It will also allow us, as policymakers, to ensure that the right measures are in place to better protect the health and safety of sex workers. I believe that it is important for any worker, regardless of the industry they work in, to have a legal framework where they can be an active participant in shaping both their rights and responsibilities. This is something I have long fought for in my professional and personal life.
+Finally, decriminalising sex work is an important step in dismantling the stigma around this industry and its workers, and this can only be a good thing. I thank all of you in the gallery for being here today. Thank you, Tammy, for reintroducing this bill and Michelle Lensink for her ongoing support, as well as those who have attempted previously to see this matter through. I particularly wish to thank Steph Key for the important role that she undertook during her time in parliament. Thank you to all who advocated on this matter for your continued energy and effort in fighting for change. I very much hope to celebrate progress and positive change with you all soon. It is time that the laws in this state are finally changed to ensure that sex worker rights are protected.
+The Hon. C.M. SCRIVEN (17:06): I rise today to speak against this bill. First, let's be clear what this is: this is the pimps' protection bill. It gives free reign to the pimps, the procurers and the profiteers who make their money from women being used. All the talk about decriminalising the women in prostitution is ignoring the fact that the people exploiting women will be the biggest beneficiaries of this bill.
+Secondly, any law that says that women can be bought is damaging to every woman in our community. It undermines the struggle for equality. It normalises violence against women. It tells men that they have a right to sexual access to women, as long as they can pay, and that women are mere products. That affects the status of every woman in society.
+Thirdly, the expected improvements for the women providing prostitution have not occurred following decriminalisation in other jurisdictions. Improvements for the brothel owners, the pimps and the men who want to buy sex—that has certainly improved—but not for the majority of women. These are some of the reasons why I cannot support the bill.
+We cannot separate the nature of the industry from a bill that intends to decriminalise the pimps and brothel owners who control it. From a narrative that says women in the industry are making free choices, the exploiters have been very successful in sanitising the industry in the public sphere and silencing the voices of the women who do speak out.
+It was referred to in the previous contribution that this is about stigma: this is not about stigma, this is about violence against women. I refer throughout this contribution to 'the women in prostitution' and this is because 95 per cent of people who provide the sex are women, but I do acknowledge that there is another 5 per cent of people involved.
+There is a plethora of academic literature on prostitution, some of which I will quote today. I have been to briefings and have spoken to lobbyists, such as the Sex Industry Network, and I have spoken to women who have been in prostitution. It is there that I would like to start, with the people who have experienced the reality of prostitution, as providers of sex over an extended time. I have spoken directly with many of the women whose stories I recount here. Some have written down and even published their experiences. It is their voices that often are not heard in this debate.
+I do alert the chamber to the fact that it might be quite difficult to listen to their experiences, and it will take some time. I hope that all members will respect the women, who have told about their trauma, enough to listen. Rhiannon grew up in Canberra and says that the brothels and strip bars have their biggest spike in business during parliamentary sitting weeks when politicians and the lobbyists are there. Prostitution is under a legalised scheme in the ACT, and she says that its reputation as a sex capital seems to make it more socially acceptable for men to buy sex.
+She explains how she became trapped in the sex trade following the GFC. She had moved to Queensland and could not get a job, and her student payment barely covered the rent. She got behind in her rent payments and was worried about eviction. She says:
+When you are a woman, especially a young and attractive one who is struggling to find work, there is one form of so-called employment that is always and ubiquitously available; the sex industry is aggressive in its pursuit. Men constantly suggested stripping and prostitution when I complained of not being able to find a job. Ads promising fast cash jumped out from newspapers. Strip bars had flashing signs out front: 'Dancers wanted for immediate start $$$'.
+After almost a year of unemployment and the stress of poverty I accepted a job as a bikini waitress. The job required me to travel to taverns and pubs that had booked me through an agency and, dressed in a G-string bikini and high heels, greet the men who entered the bar. I was required to flirt with them, take their orders and bring them drinks. I rationalised that I would be wearing a bikini if I were at the beach and that being paid more than I would as a bartender just to wear a bikini and serve drinks was almost a good thing. But I couldn't deny the reality that I was being paid to submit to the status of sexual object. I could never escape the deep sickness I felt when the eyes of those men were on my flesh.
+Women in the university feminist collective used a language of choice to talk about prostitution and stripping; 'My body, my choice.' What I was doing did not feel like bodily autonomy, it felt like I was selling my bodily autonomy. When a person is paid for sex they are being paid precisely because of the fact the sex is unwanted. Sexual autonomy cannot exist when a person is sexual for any reason outside their own desire, for their own pleasure. The sacrifice of my bodily autonomy was precisely what I was being paid for. I felt ashamed for acquiescing to sexual objectification, but also felt it wasn't me who had created the situation. Choice was the last thing I felt I had. I was unable to do the job without being drunk and, unlike any other job I had ever had, I was allowed to have the men buy me drinks and to drink as much as I wanted.
+Because there were only one or two jobs available a week—with these being only two-hour shifts, and because the agencies took half the fee, I made next to nothing. I still struggled to pay the rent. After a few weeks the agency began to tell me there were no bikini jobs that week and all that was available was lingerie waitressing at bucks' parties. It didn't seem like a huge line to cross, and I needed the money. Walking almost naked as a woman into a room full of drunk, rowdy men, many twice my age, made me feel vulnerable and shaky. They heckled and groped me and tried to photograph me. Some referred to me as 'slut' rather than use a false name I had given.
+I was always offered extra cash to remove my bra. At first I refused. One man complained his money had been wasted because he had wanted to 'see some tits'. He pulled down his pants and flashed his genitals at me yelling 'Suck it, bitch,' as I left. I'd consume several drinks before arriving and continue drinking through the shift—this was the only thing that made it possible to endure.
+After a couple of weeks the agencies told me there were few bookings for women not willing to perform a strip show using vegetables or dildos, and the only other jobs they had were for topless waitressing. The offer of more money for being bra-less, and the thought that I wouldn't be hassled and pestered to take my bra off…was enough to make me agree.
+She says:
+Society grooms women long before they enter the sex industry and the industry continues to groom us. After a few times serving men drinks in nothing but stilettos and a G-string, doing so in nothing but stilettos didn't seem like much of a line to cross. One week, when the only booking available was for a nude waitress at $20 extra an hour, I agreed to it.
+A week after that I was sent to a venue where men had ordered a naked poker dealer. I undressed and accepted a glass of whiskey. I woke a day later [in another location] with a man's shirt over me and nothing else. My body hurt inside and my thighs were bruised. I had a black eye and a near blank memory. I didn't think there was any point going to the police—the men would simply say I was drunk and had consented (I had reported a rape to police once before as a teenager and was told I had little chance of a conviction).
+The agency kept no details of the men who made bookings with them anyway, and I couldn't have tracked them down if I'd wanted to. My phone and wallet were gone and the money for the topless poker game with it, but the agency had taken their large cut of my fee with the booking so there was no loss for them.
+I called an older women I had worked with at a few bucks' nights. She had offered me Oxycodone tablets during a worse-than-usual shift. Up until then I had refused, but that day I asked her to meet me. The pills made me feel better. I bought various drugs from then on. I hitchhiked to Sydney. I had decided I would work as an escort. I felt so violated that I just didn't care any more. All I wanted was money for drugs.
+It is illegal to be prostituted as an escort in Queensland. Prostitution can only legally occur in-house at a licensed brothel, but it was legal in New South Wales. I bought into the illusion that being a high-class escort would be more palatable and highly paid, and I imagined there would be some kind of glamour in it.
+The agency advertised their call-out rates at $600 to $1,500 per hour, depending on the rank they gave you, but they took half. Plus, I would need to spend thousands on designer suits and shoes, hair and beauty procedures, including teeth bleaching, waxing and eyelash implants. I would probably need breast implants too. This was because they usually only dispatched out-of-work models. I was too short, so I was advised to at first work in less exclusive brothels to save up money for the beauty procedures.
+So, I hitchhiked back to Brisbane and went to work in a strip bar instead. I had convinced myself I didn't care what I had to do for money any more. I just didn't care about anything much at all. I could barely sleep due to nightmares. I figured working at a strip bar would distract me from them. I had also become infatuated with a heroin-addicted man, who later became abusive and violent. I needed money to support him.
+So, at the bar dancers can gyrate naked against a pole all night and still make no money. The men pay a fee of around $30, at that time, to enter, but the club keeps all of it. The women are paid only if a man chooses them for a private dance. The dancers have to compete with each other to convince the customers to choose them. The only thing more degrading than having to gyrate naked on the lap of a balding, fat, old man for money is to have to beg him to pay you to do so, while he objects that the fee is too high.
+There is a common myth that men are not allowed to touch strippers during a private dance. The truth is that the private dance usually entails the man putting his hands all over you and doing almost anything but penetrate you. The club takes at least half of the private dance fee. The man who owns the strip bar also owns several others across Brisbane that he rotated us around.
+I worked with women who had grown up in foster care, women who had fled childhood sexual abuse, women who had lived on the streets, women living with drug dependency and young single mothers who had no other way to provide for their kids. All of us had been raped at least once and some of us habitually self-mutilated. Punters never seemed to care about the scars on your wrists.
+We are told of women who love working in the sex industry, but in my time I never met such a woman. One night at the strip bar none of the men had paid me for a private dance. I had not made a cent, despite stripping to nothing and gyrating around the pole. As usual, the men refused to give me any tips because they had paid at the door. They didn't care that I got none of the door fee. I became increasingly desperate to sell a private dance, but all the men said the fee was too much, and maintained they would pay it only if I would go out the back with them for full sex. Most were old enough to be my grandfather, which only added to my disgust and feelings of degradation.
+By about 4am, when the bar was closing, I handed the red dress we were required to wear to the boss. By this point I was drunker than usual and doped up on Codeine and Xanax. I stumbled on to the street and a flood of built-up tears that could no longer be contained began to spill out. The more I cried, the more the tears flooded out. A man approached me on the almost empty street and asked if I was okay. I had lived long enough to know that the man who approaches the damsel in distress does not actually care about her. I asked him flat out would he pay me to have sex with me. He told me he had $200 and I followed him to his apartment.
+In the world I lived in the sum of all I was worth was $200. That fact filled me with more pain than I could contain. In his bathroom I took the rest of the pills left in my bag, found his razor and used it to cut my wrists, then removed my clothes and went and lay down on his bed, with blood sticking to the toilet paper I had stuck on the cuts. He only had $100 he said—it was all he could find. I insisted on clutching the cash while he used me.
+This man felt it was worth paying $100 to have sex with a woman who had a tear-stained face and bleeding wrists. When he was finished I got up, put my clothes on and calmly said, 'You need to call an ambulance now, because I'm going to kill myself'. He responded with a blank, stupefied look and kind of shrugged. I walked out of his apartment and dialled 000 myself.
+The ambulance did come. I was held at a psychiatric ward overnight; a place I have been admitted to more times than I can count. A psychiatrist told me I had Post Traumatic Stress Disorder alongside the Borderline Personality Disorder I had previously been diagnosed with. I was now eligible for a disability pension under mental health criteria. The pension is enough to live on comfortably while studying full time and, unlike other welfare payments, is reliable and long term.
+It strikes me as absurd that Australia's welfare system required me to become psychiatrically disabled by sexual abuse in order to be considered eligible to receive the amount of financial support that would have prevented much of the sexual abuse in the first place.
+Rhiannon eventually reconnected with her stepfather and moved back to live with him in Canberra. He paid for hours of group therapy sessions for her and she later returned to study in Brisbane. She said:
+The safety and comfort of being on the disability pension afforded me a sense of security I had never known. Knowing you will never have to have sex with anyone you don't wish to brings such freedom and nourishment to the body.
+I'm not telling my story in search of pity; none of us want your pity. I tell it as a testimony to the bare truth of what prostitution is, the truth that every day is drenched in lies.
+I'm telling this truth not for myself but for all the women who are still suffering and those yet to suffer in this climate of denial.
+Those who want to deny the exploitation in prostitution will find ways to say that Rhiannon's experience is not relevant, but I think it is obvious that her abuse was not caused by stigma, or legalisation instead of decriminalisation, or any of the other ways they try to discredit women's stories. It was caused by the men who demand sex and the club owners who exploit them. It was caused by the nature of the sex industry.
+Another survivor I spoke to said that support for decriminalisation was being fuelled by sex workers' rights groups who, although they represent the minority of people in prostitution, tend to be the most vocal. She said:
+The exploited, trafficked, voiceless, marginalised and most vulnerable tend not to speak up as often or as loudly. Their voices are not being heard in this discussion and they need to be.
+The status of all women is affected by misogyny and power imbalance. The question for we who are considering this bill is whether decriminalisation of the pimps and brothel owners will establish greater respect for women in our society, including those in prostitution, or less.
+A report that looked at prostitution across nine countries contrasted prostitution to non-commercial casual sex, where both people act on the basis of sexual desire and both are free to retract without economic consequence. In prostitution, there is always a power imbalance where the john, the buyer, has the social and economic power to hire her or him to act like a sexualised puppet.
+Members may or may not be aware that there are online review sites where men post reviews and rank the women with whom they have bought sex. Their attitudes to women, as revealed on these sites, is instructive, including comments such as, 'She's a sad waste of good girl flesh,' or, 'If you want an attractive receptacle for your semen she will do.'
+The Comparing Sex Buyers study by Farley et al. reveals that men who pay to sexually exploit women are aware of the harms they inflict. It found that 'two thirds of both the sex buyers and the non-sex buyers observed that a majority of women are lured, tricked or trafficked into prostitution' and that '41 per cent…of the sex buyers used women who they knew were controlled by pimps at the time they used her.' This awareness, however, did not stop them.
+This study found that sex buyers tend to regard the women they buy as less than human and as solely existing for their sexual use and enjoyment. Men who purchase sex are often quite open about their belief that their entitlement to sex should take precedence over the wellbeing of the women they buy. Common themes emerge: one is that the sex buyers regard the women they buy as mere objects for sexual gratification. They appear to despise the women they buy and require of these women absolute compliance and submission to the sex acts demanded of them.
+The Comparing Sex Buyers study crucially finds that in systems of prostitution, sex buyers are motivated by the opportunity to control and dominate a woman so that they can perform degrading sex acts against her that female partners would refuse. Farley and colleagues recorded statements from buyers such as, 'If my fiancée won't give me anal, I know someone who will,' and:
+You get to treat a ho like a ho…you can find a ho for any type of need—slapping, choking, aggressive sex beyond what your girlfriend would do—you won't do stuff to your girlfriend that will make her lose her self esteem.
+One man complained about his experience in Amsterdam. Before anyone thinks to themselves, 'What's that got to do with us?', this is about the attitudes of the men who are buying sex. He said:
+[It] was like going through a turnstile into a fairground ride: in and you're out. The idea that the women had been with five men in the last hour or 20 men in a day was a big turn off.
+Note that his concern is not that perhaps a woman servicing five men in an hour, or 20 in a day, might be suffering physical trauma or any other impact; the issue is that he found it a turn-off. Buyers believe their purchasing power entitles them to demand any type of sex they want, and this is borne out by the experiences of women who have worked in decriminalised environments. One woman who was in prostitution in Australia and New Zealand, both before and after legalisation and decriminalisation, said that, contrary to promises from the pro-prostitution lobby, punter violence—that is, buyers' violence—increased in New Zealand after the 2003 change in the law. She says:
+[In 2003] the police violence stopped overnight under decriminalisation, so on that level it was good—
+I mention that that obviously is a good outcome from decriminalisation—
+but the johns…within the space of a year the johns got more violent and had greater expectations. They thought they could do whatever they wanted, thought they had bought your body. I had never had someone say 'I paid for your body and I can do what I want' until decriminalisation.
+One of the consequences of decriminalisation in New Zealand was that brothels offer all-inclusives. This is where men pay a flat fee to come into a brothel and can then have sex with as many women as they wish and can do whatever they wish. The women have no choice and no control because it is the brothel owner who calls the shots. As I mentioned, 95 per cent of people providing sex and prostitution are women and 99 per cent of buyers are men. This is clearly a gendered issue.
+Many in this place have campaigned against the objectification of women: that the value of women and girls should not be based on their physical attractiveness and sexual appeal. It is an important principle, which is completely undermined by the promotion of prostitution. This bill proposes a system where pimps and brothel owners are totally decriminalised and there is nothing to stop the advertising of women as though they are pieces of meat on a slab, available to any person who hands over some cash.
+The rhetoric is around choice, that this is a sex worker's chosen occupation and the law should not interfere with that, yet we do restrict people's choices if they are deemed damaging. We ceased supporting grid girls after 2016 because it was deemed inappropriate and to be encouraging the objectification of women. Indeed, on 23 February 2016, the Hon. Ian Hunter replied to a question about the Body Image SA project, saying:
+The sexualisation and 'sexploitation' of women is a key issue in sport. The Minister for Recreation and Sport has indicated that the government will not continue to support the grid girls after the 2016 Clipsal race.
+So women were no longer able to choose to be involved in the sexualisation and sexploitation of women as grid girls because of its effects on the status of women in general. There is a strong campaign at present, which I support, to get rid of Wicked Campers on our roads because of their vile misogynist messages about women and the way that seeing such messages can shape the attitudes of boys and men towards women.
+We rightly rally against the objectification of women. We condemn misogynist slogans. We encourage our girls to see their value as more than just their sexual appeal, but are we then going to decriminalise the people who profit from women's prostitution? One woman wrote:
+For the rest of you, I want you to know that the vast majority of people working in prostitution are not consenting adults who, feeling empowered by a plethora of other employment options, decide that selling their bodies for sex is their most desirable career.
+Prostitution turns people into products. Inherently, it is built on systems of gender inequality where women are dehumanized and sexually exploited for the pleasure and gratification of men. This is evident in the fact that 98% of those being bought are women and 99% of those buying sex are men.
+Ultimately, it is not a system of empowerment but one that exploits those with the least power. Some women call this the pimp protection bill and say:
+…the legalized buying and selling of women is in effect the promotion of and profiting from women's poverty, childhood sexual abuse, sexual harassment and sexual exploitation.
+I spoke to several women who had campaigned for decriminalisation, but when it actually happened they saw its devastating effects and changed their minds. Wherever prostitution is legal the demand for commercial sex increases, which provides a great incentive to pimps and sex traffickers to push more women into the marketplace to sell. We saw from the earlier story that someone can start by simply wanting to work in a bar because of their poverty and end up in a place that they certainly have not</t>
+  </si>
+  <si>
+    <t>Answers to Questions</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-11-34466</t>
+  </si>
+  <si>
+    <t>The Hon. T.J. WHETSTONE (Chaffey—Minister for Primary Industries and Regional Development): The following details for purchases of alcohol by the Office of the Minister for Primary Industries and Regional Development which have been reimbursed:</t>
+  </si>
+  <si>
+    <t>Ministerial Expenditure</t>
+  </si>
+  <si>
+    <t>Building Better Schools Program</t>
+  </si>
+  <si>
+    <t>115 Dr CLOSE (Port Adelaide—Deputy Leader of the Opposition) (24 July 2018). Can the minister guarantee that Charles Campbell College will receive $11 minister under the Building Better Schools Infrastructure Program and be able to progress with plans to build new flexible learning areas, relocating sports playing courts and trade training centre and replacing the administration block with a nature play area, as outlined on the Department for Education and Child Development's website?
+The Hon. J.A.W. GARDNER (Morialta—Minister for Education): I have been advised of the following:
+The government proposes to deliver this school's Building Better Schools project in line with the announced dollar value as described.
+The illustrations and lists of desired improvements prepared for all schools in the program clearly stated 'These initial plans are subject to further planning and may change'. This statement was placed under the illustration when the former government was in power as the allocation to each school was determined before the scoping documents were commenced. Neither the former government nor the Department for Education ever provided any guarantee that each school's aspirations could be met in total.
+The work currently being undertaken by the Department for Education in collaboration with this school will determine the detail of the final project (or projects) that will go ahead. The guiding principles for the work, developed under the former government, when the Member for Port Adelaide was the minister, and then published in each school's brochure in February 2018 remain:
+the removal of old relocatable or modular classrooms
+creation of new buildings for schools with growing student numbers
+the refurbishment of classrooms and building, transforming then into modern learning areas
+landscaping and upgrades of the street frontage.</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-11-30661</t>
+  </si>
+  <si>
+    <t>Drinking Water Quality</t>
+  </si>
+  <si>
+    <t>The Hon. S.G. WADE (Minister for Health and Wellbeing): The Minister for Environment and Water has been advised:
+1. Under the Safe Drinking Water Act 2011, any plans developed by SA Water for monitoring drinking water supplies, including testing of reservoir waters, have to be approved by SA Health. SA Water has advised that the proposed review of existing laboratory services will not reduce monitoring capabilities, including testing of reservoir waters.
+In addition, in line with government commitments, the opening of reservoirs for recreational access will be undertaken in a manner that protects the safety of drinking water supplies and ensures compliance with the requirements of the Safe Drinking Water Act 2011.
+To support these commitments, SA Health is leading a public health risk assessment in conjunction with SA Water and the Department for Environment and Water to identify which recreational activities can be introduced with low risk to drinking water safety.
+2. SA Water has advised SA Health about a proposed restructure of its operations in a business unit. This restructure is currently the subject of consultation.
+I am advised that this proposed restructure relates to the loss of an interstate water testing contract. I am advised that any staff changes that may occur through this restructure will not compromise existing water quality testing or public health, ensuring that the skills and expertise required to meet public health responsibilities are maintained. Any suggestion of water quality being jeopardised as a result of these proposed changes is incorrect and misinformed.</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-10-26776</t>
+  </si>
+  <si>
+    <t>Lymphoedema</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-11-33921</t>
+  </si>
+  <si>
+    <t>The Hon. D.C. VAN HOLST PELLEKAAN (Stuart—Minister for Energy and Mining): The Minister for Health and Wellbeing has been advised that:
+It is not possible to accurately advise the number of people who have a lymphoedema condition in the electorate of Frome and surrounding areas. Country Health SA does not keep a database of lymphoedema patients. Many patients are treated in primary health settings by private physiotherapists and/or their general practitioner.
+The Port Pirie GP Plus services reports ten patients with lymphoedema are currently receiving outpatient services including massage therapy. Seven people with lymphoedema are waiting for outpatient services.</t>
+  </si>
+  <si>
+    <t>SA Health</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-10-23279</t>
+  </si>
+  <si>
+    <t>4 The Hon. K.J. MAHER (Leader of the Opposition) (16 May 2018).
+1. What open application and assessment process occurred prior to the hiring of the new SA Health chief executive officer?
+2. Did the minister have any discussions with Mr Chris McGowan about hiring him as the new chief executive of SA Health before the state election?
+3. Did the minister have any discussions with the Premier about hiring Mr Chris McGowan as the new chief executive of SA Health before the state election?
+4. Did the minister have any discussions with any public servants about hiring Mr Chris McGowan as the new chief executive of SA Health before the state election?
+5. Did the minister have any discussions with anyone at all about hiring Mr Chris McGowan as the new chief executive of SA Health before the state election?
+6. Has the minister or the Premier given requests to SA Health about the hiring or dismissal of any employees except for the chief executive?
+The Hon. S.G. WADE (Minister for Health and Wellbeing):
+1. Dr McGowan was one of several candidates interviewed for the position in a process that has been used by previous governments for such an appointment. He was recommended based on his skills and extensive experience in the health sector.
+2. The government was not in a position to offer anyone the position until after it was sworn in on 22 March
+3. I am not accountable to the house for any private discussions I may have had with any of my parliamentary colleagues prior to the swearing in of the government on 22 March.
+4. I am not accountable to the house for any private discussions I may have had with any public servants prior to the swearing in of the government on 22 March.
+5. I am not accountable to the house for any private discussions I may have had with any person prior to being sworn in as minister on 22 March
+6. Neither the Premier nor I have given any requests to SA Health about the hiring or dismissal of any employee by SA Health except for discussions focused on the staffing of, and support for, my ministerial office.</t>
+  </si>
+  <si>
+    <t>Modbury Hospital</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-10-23278</t>
+  </si>
+  <si>
+    <t>3 The Hon. K.J. MAHER (Leader of the Opposition) (15 May 2018).
+1. Did SA Health provide any advice whatsoever indicating that a stand-alone high dependency unit (HDU) at Modbury Hospital could lead to unsafe patient outcomes? If so, what was the nature of the advice?
+2. Will a stand-alone HDU at Modbury Hospital receive accreditation from the College of Intensive Care Medicine of Australia and New Zealand?
+3. Has the minister received any advice whatsoever regarding a stand-alone HDU receiving accreditation from the College of Intensive Care Medicine of Australia and New Zealand?
+4. Will the minister guarantee that 24/7 cardiac emergency services will be restored at The QEH within 100 days, as outlined in the Liberal Party's election commitment?
+5. Can the minister guarantee that no clinical services will be removed from The QEH?
+6. Did the minister receive any advice whatsoever showing that signing up to the Federal National Health Agreement would deliver a worse outcome for South Australia than the previously signed Federal Hospital Funding Agreement?
+7. What are the projections for funding to be received by SA under the new Federal National Hospital Agreement compared to the original agreement?
+8. Can the minister guarantee that no services will be removed from any country hospitals?
+9. Which elective surgery procedures will be performed at the reopened Repat as per the Liberal Party election commitment?
+10. How many additional hospital beds will be opened as part of the winter demand management for 2018, and at which hospitals?
+The Hon. S.G. WADE (Minister for Health and Wellbeing): I have been advised:
+1. I can confirm I received advice from SA Health indicating in the absence of establishing a new intensive care unit at Modbury Hospital, appropriate levels of clinical safety may not be achieved with the establishment of a stand-alone high dependency unit.
+2. That is a matter for the College of Intensive Care Medicine of Australia and New Zealand if and when accreditation is sought.
+3. I can confirm that I have received advice from SA Health indicating accreditation from the College of Intensive Care Medicine of Australia and New Zealand would be unlikely with the establishment of a high dependency unit without appropriate intensive care unit support.
+4. Work is on track to meet the government’s commitment to ensure TQEH has the capacity to deal with cardiac emergencies 24 hours a day, seven days a week within the government’s first 100 days.
+5. All decisions relating to clinical services are made on the basis on patient safety and clinical need.
+6. South Australia has not yet signed up to a new national health agreement. What the Premier signed in April this year was the heads of agreement between the commonwealth and the states and territories on public hospital funding and health reform (the heads of agreement). What the heads of agreement does not do is outline specific funding allocations to any jurisdiction.
+7. As the new national health agreement is still in the process of being negotiated, the government is not yet in a position to make any direct comparisons between the existing and new funding arrangements and levels.
+8. The Marshall government has a longstanding commitment to country hospitals and health services. There is a large focus by this government on country South Australia as we move to local level decision-making and the establishment of boards and separate regional health networks.
+Other key commitments regarding country health include:
+investing in country hospitals by addressing the backlog of capital works, as well as several specific commitments to regional and country hospitals;
+increasing the level of chemotherapy being delivered in country South Australia;
+developing and implementing a rural health workforce plan.
+9. SA Health is currently in the process of identifying opportunities for public health services at the Repat site based on asset functionality, with the use of elective facilities a key component of this planning.
+10. The Department for Health and Wellbeing does not commission or fund beds. Acute activity is funded based on separations and a target length of stay. Hospitals have the ability to increase the bed base to cater for increased demand.</t>
+  </si>
+  <si>
+    <t>Health Services</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-11-32755</t>
+  </si>
+  <si>
+    <t>540 Mr PICTON (Kaurna) (13 February 2018). What are the FTEs across our health services, for 2016- 17, for 2017-18, budgeted costs for this financial year and over the forward estimates, broken down into the following categories—DHW employees, LHNs, SAAS, medical professionals, nursing/midwifery, allied health professionals, public sector salaried officers, public sector executives, grant-funded scientists, medical scientists, technical officers, weekly paid/metal trades, dental officers, SA Ambulance Award, ministerial appointments and principal research fellows?
+The Hon. D.C. VAN HOLST PELLEKAAN (Stuart—Minister for Energy and Mining): The Minister for Health and Wellbeing has advised:
+I refer the member to the evidence given to the South Australian Parliamentary Committee on Occupational Safety, Rehabilitation and Compensation's inquiry into Workplace Fatigue and Bullying in south Australian Hospitals and Health Services on Friday 7 December 2018.</t>
+  </si>
+  <si>
+    <t>Influenza Vacinations</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-10-23286</t>
+  </si>
+  <si>
+    <t>The Hon. K.J. MAHER (Leader of the Opposition) (29 May 2018). On what date did the minister request that the Chief Medical Officer purchase flu vaccine supplies to provide to 0-5-year-old South Australians? In what form was this request?
+The Hon. S.G. WADE (Minister for Health and Wellbeing): As I informed the council on 8 May 2018, I did not request that the Chief Medical Officer purchase flu vaccine supplies. My response at that time was:
+"The fact of the matter is I have had discussions with the Chief Medical Officer. The Chief Medical Officer has said that he has been able to secure supplies. I didn't order him to put the order in; I am very glad he did." (p.53)
+I am advised that the first order for flu vaccine stock for the South Australian influenza program for all children aged 6 months to less than five years of age was placed with the manufacturer on 23 April 2018.
+There had been inquiries and correspondence prior to the change in government about the possibility of such a program and at that time the advice from vaccine manufacturers was that there was insufficient supply to support such a program.</t>
+  </si>
+  <si>
+    <t>Flinders Medical Centre</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-10-23290</t>
+  </si>
+  <si>
+    <t>The Hon. K.J. MAHER (Leader of the Opposition) (29 May 2018). Is the government committed to the existing capital works scope and budget for the redevelopment underway at Flinders Medical Centre and if not, what changes have been made?
+The Hon. S.G. WADE (Minister for Health and Wellbeing): I have been advised:
+The government remains committed to the capital works at the Flinders Medical Centre (FMC).
+The recent $185.5 million FMC redevelopment project provided a new multilevel car park, a new rehabilitation and palliative care building and a new older persons mental health facility. These facilities are fully completed and operational and are now within a defects liability period.
+The $17.5 million FMC neonatal unit redevelopment project which will provide an upgraded and expanded neo natal unit remains in construction. This project is forecast for completion in September 2018.
+During late 2017, the two existing cold shell operating theatre spaces at FMC were fully fitted out including the installation of specialist medical equipment within the approved capital budget of $3.5 million. These works are fully completed and operational and are now within a defects liability period.</t>
+  </si>
+  <si>
+    <t>Nuclear Waste</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-10-23311</t>
+  </si>
+  <si>
+    <t>In reply to the Hon. M.C. PARNELL (15 May 2018).
+The Hon. D.W. RIDGWAY (Minister for Trade, Tourism and Investment): I have been advised:
+1. No.
+2. No. In considering this matter the government has been guided by the Nuclear Fuel Cycle Royal Commission Report which considered the potential impact on tourism from the establishment of an international radioactive waste management facility and advised the impact on tourism would be inconsequential.</t>
+  </si>
+  <si>
+    <t>Auditor-General Controls Opinion</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-11-32619</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In reply to the Hon. S.C. MULLIGHAN (Lee) (28 November 2018).
+The Hon. S.S. MARSHALL (Dunstan—Premier): I have been advised:
+From 2018-19, the Auditor-General will be undertaking a risk-based approach when forming his controls opinion at a whole-of-government level.
+This means the Auditor-General will be focusing on public sector agencies that present the most material exposures at a whole-of-government level ie. areas that have the most quantitative and qualitative significance.
+Based on initial feedback from the Auditor-General's office the Department of the Premier and Cabinet (DPC) is not one of the agencies that is being prioritised to form a controls opinion at a whole-of-government level. This is largely due to the recent machinery of government changes which have resulted in DPC being a much smaller agency than it was in previous years.
+</t>
+  </si>
+  <si>
+    <t>Auditor-General's Report</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-11-32795</t>
+  </si>
+  <si>
+    <t>In reply to the Hon. A. KOUTSANTONIS (West Torrens) (14 November 2018).
+The Hon. V.A. CHAPMAN (Bragg—Deputy Premier, Attorney-General): I indicated that my understanding was that 'some kind of memorandum' went from the Attorney-General's Office to the Treasurer and/or to SAicorp with respect to arranging payment of $2.57 million.
+Having reviewed materials, I confirm that the Crown Solicitor's Office wrote to SAicorp on 1 May 2018.
+I am advised that the Auditor-General did not request any cabinet documents, cabinet submissions or cabinet notes regarding the payment.</t>
+  </si>
+  <si>
+    <t>In reply to the Hon. K.J. MAHER (Leader of the Opposition) (13 November 2018).
+The Hon. S.G. WADE (Minister for Health and Wellbeing): I have been advised:
+Yes.</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-10-26307</t>
+  </si>
+  <si>
+    <t>In reply to Mr MALINAUSKAS (Croydon—Leader of the Opposition) (28 November 2018).
+The Hon. S.S. MARSHALL (Dunstan—Premier): I have been advised:
+The increase in the Urban Renewal Authority's core debt facility was approved by the Minister for Transport, Infrastructure and Local Government and the Treasurer.
+Section 21(4) of the Urban Renewal Act 1995 requires that increases in the core debt limit by the Urban Renewal Authority are approved by the minister responsible for the Urban Renewal Authority, not a minister responsible for any particular project the Urban Renewal Authority may undertake.</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-11-32954</t>
+  </si>
+  <si>
+    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-11-32797</t>
+  </si>
+  <si>
+    <t>In reply to Ms STINSON (Badcoe) (28 November 2018).
+The Hon. R. SANDERSON (Adelaide—Minister for Child Protection): I have been advised:
+Pursuant to section 110A(2) of the Children and Young People (Safety) Act 2017 (CYPS Act)and regulation 34 of the Children and Young People (Safety) Regulations 2017 (CYPS Regulations), persons working in residential facilities established under the Family and Community Services Act 1972 who are not employees of the Department for Child Protection (i.e. NGO and commercial care staff and volunteers) will be required to undergo psychological assessment by 6 September 2019.
+Pursuant to section 107 of the CYPS Act and regulation 31 of the CYPS Regulations persons employed in a licensed children's residential facility are required to undergo a psychological assessment by 22 April 2020.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +727,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF444444"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,7 +757,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -151,6 +772,9 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -466,21 +1090,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E2EC93-960C-48F4-A506-84E0208EB621}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -491,13 +1116,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>43523</v>
       </c>
@@ -508,103 +1136,359 @@
         <v>2</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>43523</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>43677</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>43678</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>43621</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="E6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>43648</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>43712</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>43601</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>43601</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>43635</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>43635</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>43508</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>43635</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>43635</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>43635</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>43440</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>43508</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>43557</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>43510</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>43508</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" location="/docid/HANSARD-11-33034" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-33034" xr:uid="{CF7EEAFE-37A7-4A68-8BFC-83188235D4C6}"/>
-    <hyperlink ref="E3" r:id="rId2" location="/docid/HANSARD-10-26906" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26906" xr:uid="{E852C2AD-6FE3-4882-8137-43B1A4DF1244}"/>
-    <hyperlink ref="E4" r:id="rId3" location="/docid/HANSARD-11-34810" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-34810" xr:uid="{60BD940E-0B70-4EE5-AF87-1AE4F8251902}"/>
-    <hyperlink ref="E5" r:id="rId4" location="/docid/HANSARD-11-34872" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-34872" xr:uid="{52962164-55D7-4F46-B5FD-E6AA6DB58035}"/>
-    <hyperlink ref="E6" r:id="rId5" location="/docid/HANSARD-10-26904" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26904" xr:uid="{67034CF3-F99C-49AB-9556-C1D5087401F6}"/>
+    <hyperlink ref="F2" r:id="rId1" location="/docid/HANSARD-11-33034" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-33034" xr:uid="{CF7EEAFE-37A7-4A68-8BFC-83188235D4C6}"/>
+    <hyperlink ref="F3" r:id="rId2" location="/docid/HANSARD-10-26906" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26906" xr:uid="{E852C2AD-6FE3-4882-8137-43B1A4DF1244}"/>
+    <hyperlink ref="F4" r:id="rId3" location="/docid/HANSARD-11-34810" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-34810" xr:uid="{60BD940E-0B70-4EE5-AF87-1AE4F8251902}"/>
+    <hyperlink ref="F5" r:id="rId4" location="/docid/HANSARD-11-34872" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-34872" xr:uid="{52962164-55D7-4F46-B5FD-E6AA6DB58035}"/>
+    <hyperlink ref="F6" r:id="rId5" location="/docid/HANSARD-10-26904" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26904" xr:uid="{67034CF3-F99C-49AB-9556-C1D5087401F6}"/>
+    <hyperlink ref="F7" r:id="rId6" location="/docid/HANSARD-11-34466" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-34466" xr:uid="{0E91C013-3D9E-4F7D-85C5-A91B67C232EC}"/>
+    <hyperlink ref="F8" r:id="rId7" location="/docid/HANSARD-11-30661" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-30661" xr:uid="{702D05ED-05E6-461B-A612-AF73132F6FEC}"/>
+    <hyperlink ref="F9" r:id="rId8" location="/docid/HANSARD-10-26776" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26776" xr:uid="{717B5977-7B99-4BBA-8546-6F0293E2CB2D}"/>
+    <hyperlink ref="F10" r:id="rId9" location="/docid/HANSARD-11-33921" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-33921" xr:uid="{0FD9BB4C-B3CB-41B9-8B06-F3BAB6A7EE13}"/>
+    <hyperlink ref="F11" r:id="rId10" location="/docid/HANSARD-10-23279" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23279" xr:uid="{883ACBE4-87FE-43D8-84D9-D07334278DF1}"/>
+    <hyperlink ref="F12" r:id="rId11" location="/docid/HANSARD-10-23278" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23278" xr:uid="{73A3AD8E-5A9A-4FA9-AE35-3861574BB535}"/>
+    <hyperlink ref="F13" r:id="rId12" location="/docid/HANSARD-11-32755" xr:uid="{9BBE697E-7419-4F79-AC17-9A6ED5A7F9AF}"/>
+    <hyperlink ref="F14" r:id="rId13" location="/docid/HANSARD-10-23286" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23286" xr:uid="{D5E612D2-F917-4A06-A220-DA369BD0FC90}"/>
+    <hyperlink ref="F15" r:id="rId14" location="/docid/HANSARD-10-23290" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23290" xr:uid="{F6621F6B-BCEF-4586-AB26-109836F94128}"/>
+    <hyperlink ref="F16" r:id="rId15" location="/docid/HANSARD-10-23311" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23311" xr:uid="{955E183C-87B2-420F-85FD-B500A0537C06}"/>
+    <hyperlink ref="F17" r:id="rId16" location="/docid/HANSARD-11-32619" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-32619" xr:uid="{CDECA91D-9FCC-4506-9583-C5970EA4CDB6}"/>
+    <hyperlink ref="F18" r:id="rId17" location="/docid/HANSARD-11-32795" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-32795" xr:uid="{5142684D-AB52-459A-9453-7743A8F7BCF3}"/>
+    <hyperlink ref="F19" r:id="rId18" location="/docid/HANSARD-10-26307" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26307" xr:uid="{A6C8D112-203F-4AD7-BEA0-8C6AD9BDF709}"/>
+    <hyperlink ref="F20" r:id="rId19" location="/docid/HANSARD-11-32954" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-32954" xr:uid="{97BEC237-75A0-4245-A3E3-292074640C85}"/>
+    <hyperlink ref="F21" r:id="rId20" location="/docid/HANSARD-11-32797" display="/docid/HANSARD-11-32797" xr:uid="{3DAE44B1-0FA3-4B6D-98FA-56AF11AEE7FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added notes to dashboards describing their limitations. Removed Motions record from dummy data. Created Client treemap.
</commit_message>
<xml_diff>
--- a/dashboard/DummyData.xlsx
+++ b/dashboard/DummyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\2015-2019 - Master of Data Science\2019-S2 - Capstone Professional Project\Project Code\dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA128D7C-7535-4FDB-98B4-1F63CA3236C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAB6EC4-CE98-41DB-8107-6D7B7EE8D755}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E3927FDB-01BF-4B08-B8D1-941CE14D3EB4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="member" localSheetId="0">Sheet1!$D$7</definedName>
+    <definedName name="member" localSheetId="0">Sheet1!$D$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -42,19 +42,10 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Motions</t>
-  </si>
-  <si>
-    <t>Defence Shipbuilding</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
     <t>Link</t>
-  </si>
-  <si>
-    <t>http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx#/docid/HANSARD-11-33034</t>
   </si>
   <si>
     <t>Bills</t>
@@ -326,83 +317,6 @@
 Debate adjourned on motion of Mr Pederick.</t>
   </si>
   <si>
-    <t xml:space="preserve">Mr COWDREY (Colton) (11:31): I move:
-That this house—
-(a) welcomes the federal Liberal government's commitment to the $90 billion shipbuilding program, which will secure the future of South Australia's defence industry for decades;
-(b) notes the significant work being undertaken by the South Australian government to ensure that South Australians can reap the maximum benefit of the shipbuilding program; and
-(c) notes the significant negative impacts on the current workforce as a result of the former federal Labor government's failure to progress any future shipbuilding contracts during its last term in office.
-Together, we stand on the brink of a never before seen flow of work into South Australia. The only reason for this work coming is that the federal Liberal government has committed $90 billion of taxpayers' money over the coming decade to modernise and strengthen Australia's naval forces, which will build a strong and sustainable sovereign Australian shipbuilding industry.
-'Sustainable' is the key word that those opposite seem to have a tough time coming to grips with. Let us never forget that, during the Rudd-Gillard-Rudd federal Labor quagmire, zero—yes, zero, nought—vessels were commissioned, causing a massive hiatus in the work done at Osborne. Too often, those opposite conveniently forget that fact. In contrast, 54 separate vessels have been commissioned by the federal Liberal government. They will create a huge amount of work coming right here to South Australia, and particularly in the western suburbs of Adelaide, in which the electorate of Colton sits. This work will be here for generations to come and that is very good news for the people of our great state.
-Currently, two offshore patrol vessels are being built by ASC Shipbuilding, with production directly employing up to 400 workers at Osborne and sustaining 600 indirect jobs. In addition, the redevelopment of the Osborne South Shipyard, a colossal structure where the Hunter class frigates will be assembled, is underway. In parallel, the Naval Shipbuilding College is also well underway. This is just the beginning. Naval shipbuilding is set to deliver an unparalleled economic benefit to our state. Around 5,200 direct jobs will be created through naval shipbuilding activities in South Australia plus more in the supply chain, the training sector, the education sector and other associated opportunities.
-The next chapter in this book of good news is the landmark contract to build 12 Attack class submarines here in South Australia, a $50 billion project. The Attack class submarines project is the largest defence procurement in our nation's history, which is something we should all be very proud of. The project will set a number of national firsts in scale, in size, in complexity and in duration.
-Earlier this month, the Premier attended the Strategic Partnering Agreement signing in Canberra, where the agreement between the Australian government and the Naval Group was formalised. To date, work on the submarines had taken place under the design and mobilisation contract. The signing is a key step in the procurement process, with the agreement representing the contractual basis to the Attack class submarines project. The $35 billion Hunter class—
-Mr Malinauskas: What is the local content requirement?
-The SPEAKER: The Leader of the Opposition is called to order for interjecting something about local content.
-Mr COWDREY: —frigate program, which will deliver nine antisubmarine frigates to the Royal Australian Navy, will create and sustain 1,500 direct jobs. In addition, 600 jobs are needed for the redevelopment of the Osborne South Shipyard and opportunities through that supply chain. These opportunities include many South Australian-based businesses—for instance, structural steel for the mammoth shipyard has been sourced by South Australian-based steelmaker, Liberty OneSteel in Whyalla. The opportunities around naval shipbuilding are not just in Osborne, Port Adelaide or more broadly in the western suburbs of Adelaide, or at Lot Fourteen. No, the opportunities that a strong and sustainable naval shipbuilding program provides will have positive impacts and flow-ons throughout our regions and our state.
-The Defence Landing Pad, to be located in Adelaide's new innovation neighbourhood at Lot Fourteen, will provide a home for global companies to develop their Australian business strategies and plan local operations. It will add to our already thriving prime and associated contractor environment a new one-stop shop supporting international defence companies to establish in South Australia that will drive defence industry investment. The Defence Landing Pad will enable international businesses to build relationships with South Australian businesses and create opportunities for our supply chain collaboration.
-This is just one example of what the Marshall Liberal government is focused on: ensuring that we as a state make the most of the significant opportunity and investment that the federal government has made in naval shipbuilding here in South Australia. It is our obligation and our responsibility to ensure that we build capability, that we as a state make ourselves known for these skills and these industries and in the future seek further opportunities so that the impact of these investments lasts far beyond the already committed works.
-The Minister for Industry and Skills tells us, sometimes ad nauseam, about the 20,800 new apprenticeships and traineeships, but the program is incredibly important. It is important because we need to work hard and make sure that we have the requisite skills in place to deliver on these projects. It is an incredible opportunity for our young South Australians, our next generation. They have an opportunity that those before them did not.
-The Marshall Liberal government is committed to maximising the local benefits of this huge investment into our state and, as I said, this includes ensuring that we have the skilled workforce needed to deliver this project. Investing in training equipment like welding simulators and providing funding for additional work-based apprenticeships will help us create the skilled workforce that is required to fully capitalise on the naval shipbuilding program.
-As I mentioned, the Naval Shipbuilding College, a fantastic new facility, is also underway and will play an important part in preparing our state for the jobs of the future and the skills that we need for our future. In addition to new apprenticeships and new traineeships, the Marshall Liberal government is also introducing the following measures to further develop South Australia's skilled workforce. We are working with industry to strengthen South Australia's VET system, including giving industry a stronger voice through the re-establishment of industry skills councils.
-We are reforming the subsidised training list so that it is guided by industry and opening up funding contestability. We are establishing a new technical college in Adelaide's western suburbs, with a focus on defence and naval shipbuilding. The opportunities naval shipbuilding presents are not limited to advanced manufacturing, to engineering, to project management or to the trade sectors. 
-Just yesterday it was reported that the education and research sector is also already seeing benefits. It was reported that Adelaide University, Flinders University and the University of South Australia have signed an agreement with French company Naval Group, working on the subs, and France's National Centre for Scientific Research to fund an international research laboratory in Adelaide. The research lab will work on artificial intelligence, autonomous systems and ergonomics, also known as human factors. It is reported that Lot Fourteen, on the old Royal Adelaide Hospital site in the Adelaide CBD, is likely to play host to the lab, with hubs expected to be placed at each of the universities.
-All vice-chancellors of the three universities are supporting this announcement. The Vice-Chancellor of the University of Adelaide, Professor Peter Rathjen, said that he welcomed further collaboration with CNRS, Naval Group and the defence industry. The Vice-Chancellor of Flinders University, Professor Colin Stirling, said that Adelaide was an ideal location for the laboratory. The Vice-Chancellor of University of South Australia, Professor David Lloyd, also welcomed the collaboration. Quite frankly, this level of collaboration between our universities is unheard of. The scale and breadth demonstrate the opportunities associated with naval shipbuilding and the commitment that the federal Liberal government has made.
-Sadly, due to the federal Labor inaction I mentioned earlier, the Australian government has had to put in place, and backdate to 1 July 2018, the ASC Shipbuilding Structural Adjustment Program to support workers who, unfortunately, have been made redundant. Through this program, workers and their partners from ASC Shipbuilding or an affected supply chain business are supported through immediate access to intensive employment opportunities through Jobactive employment providers, including job search, résumé preparation, preparation for interviews, retaining, self-help facilities, skills assessments and career advice workshops. In addition, they have been provided with assistance by way of a $2,000 employment fund to assist workers to retain and obtain licences and tickets, as well as relocation assistance, if it is required.
-As a member of this place, as a Liberal, as a South Australian and as a proud member of the western suburbs, I am incredibly proud of the commitment that the federal government has made by way of naval shipbuilding here in South Australia. I am incredibly proud to be part of the Marshall Liberal government, which is ensuring that we make the most of these opportunities for our local community and for our state.
-Mr MALINAUSKAS (Croydon—Leader of the Opposition) (11:42): I move to amend the motion, as follows:
-Delete paragraphs (a), (b) and (c) and substitute the following:
-(a) welcomes the 2016 defence white paper and the 2017 Naval Shipbuilding Plan and its commitment to developing a national naval shipbuilding capability;
-(b) calls on the federal government to secure a guaranteed level of Australian content in current and future shipbuilding programs to ensure the development of a national naval shipbuilding capability; and
-(c) calls for an independent naval shipbuilding authority to oversee the level of Australian content in future shipbuilding programs.
-Over the years, all of us in this chamber have heard ad nauseam the sort of speech just given by the member for Colton. More recently, the South Australian public has become accustomed to both sides of politics trying to claim credit for the fact that we now have an extraordinary opportunity coming our way in the form of the submarine program, with the Future Submarines being built here in South Australia. Truth be told, both sides of politics have had a hand in this exercise. We know that, if it were not for the ferocious campaigning and fighting for our state, the Future Submarines build was going to Japan. That is now a commonly accepted fact.
-Equally, we also know that on the back of that pressure coming from state and federal Labor, it was ultimately a federal conservative government that changed their tune on sending the work to Japan and instead opted for a sovereign capability here in Australia, with the Future Submarines being built in Australia by the Naval Group.
-So let's dispense with the tired old arguments around who can claim credit for what in regard to future sub builds. Instead, let's just focus on what is actually going to happen for our state in the future because I think we are all very cognisant of the fact that this is now an extraordinary opportunity. This is not just a once in one generation opportunity but a once in multiple generations opportunity. This is not likely to be something that we are going to see come to our state again in the future. We must make sure that we do everything that is humanly possible to maximise the opportunity for this state and all the chances for jobs that are coming our way.
-What we have seen over the last fortnight is a dropping of the ball when it comes to ensuring the delivery of jobs for our economy, because what we know is there is a legitimate contest. It will not surprise people that in France they view the awarding of the submarines contract to Naval as an extraordinary opportunity for the French economy. The Naval Group is celebrating this as a boon for French jobs. French politicians are celebrating this as a winning of the industrial Olympics for France. 
-So quite understandably, quite rationally, quite pragmatically, the French will do everything they can to maximise the opportunity of this $50 billion Australian investment delivering for French jobs. It is equally important that we as a nation and that we as a state acknowledge that legitimate competition and do everything within our power to ensure that jobs will be delivered here in South Australia.
-As the member for Colton referred to in his remarks a bit over a fortnight ago or thereabouts, a very important contract signing occurred interstate between the Commonwealth of Australia and the Naval Group: the strategic partnership agreement. The federal Minister for Defence, minister Pyne, was present, obviously, for the signing. Indeed, the Premier flew over for this photo opportunity. This event seemed to fly below the radar. One would have thought that the signing of the single biggest strategic partnership agreement for the largest procurement that our nation has ever entered into would have received a little more fanfare than just a singular quiet photo opportunity.
-Quite a few of us in state and federal Labor were taken a little aback that there was not much fanfare associated with such a significant event, and now we are starting to learn why. As information has started to filter out about this strategic partnership agreement, we have learned that there are some very real and legitimate concerns about whether or not that agreement is going to deliver the level of local procurement that all of us in South Australia want to see and whether or not it is going to deliver the real jobs that we have been promised. Let's just have a quick look at the historical context.
-With the Collins class submarine, the current class built here in South Australia on the back of advocacy from state Labor and delivered ultimately by federal Labor—but put that aside—we know that approximately 70 per cent of all the work that has occurred on the Collins class submarine has been done with local content. Look at another program: the Anzac class of frigates. We know that they have delivered about 80 per cent of local content for Australia.
-So where are we at with the submarines—the future build—the largest ever capital project that the Commonwealth of Australia has ever entered into since Federation? What is the local procurement requirement in the strategic partnership agreement? What is the minimum local content standard? Well, we have learned that there is none—none. There is no local content requirement in the strategic partnership agreement from the information that we have garnered through forensic inquiries made in the Senate estimates process.
-If that does not have everybody alarmed about how many jobs are actually going to come our way, then I am not too sure what will. Yes, it is true that there are clearly going to be jobs from the submarine build in South Australia, but are we maximising this opportunity? Are we doing everything we can? Where was the Premier's advocacy, where was this government's advocacy, in trying to secure a local content requirement?
-We have heard nothing. We have heard nothing but complete silence, and that is borne out by the fact that there is no local content requirement within this agreement. There are plenty of people in local industry who are genuinely concerned about this, as well they should be. We know that if you are going to have a local content requirement in such a contract, it would exist in this one. That is what the pundits tell us. That is what one would reasonably expect—that an agreement of such importance would contain some reference to local content, yet we know there is none.
-Of course, this comes on the back of some pretty large promises that have been made by the conservative side of politics when it comes to local content. We know that a 90 per cent number was thrown around that people were trying to have an association with. We know that minister Pyne himself referred to 60 per cent plus local content. In December last year, minister Pyne said that these jobs would be delivered through an assured level of local content. He told journalists, 'This will be a local build. A local build is defined as being around 60 per cent plus.'
-So we expect this to be a local build, yet we find out what the Strategic Partnering Agreement actually says: nothing. It is utterly delusional for anyone in this place, particularly people who are responsible from the party or the government, to suggest that they can now guarantee that 60 per cent figure when the very agreement that underpins this contract has no reference to local content. What guarantees and assurances can the Premier of this state or the member for Colton give the people of South Australia that we are doing everything we can to maximise this opportunity? None, it turns out—none.
-It is starting to demonstrate a bit of a pattern in the way this government behaves when dealing with the Commonwealth of Australia. It turns out that the modus operandi of this conservative Liberal government is to take their orders from their conservative Liberal mates. We have seen it on the Murray, the way they sold us out of our 450 gigalitres of upwater, and now we have seen it on the most important opportunity that this state has ever had in its history: being able to build the single largest procurement engagement exercise that has ever occurred in the history of Federation. Let it be known that on this side of the chamber we will do everything we can to fight for South Australian jobs, not capitulate and kowtow to their masters in Canberra.
-Mr BROWN: Mr Deputy Speaker, I draw your attention to the state of the house.
-A quorum having been formed:
-Mr McBRIDE (MacKillop) (11:53): I rise to speak in support of the motion put by the member for Colton:
-That this house—
-(a) welcomes the federal Liberal government's commitment to the $90 billion shipbuilding program, which will secure the future of South Australia's defence industry for decades;
-(b) notes the significant work being undertaken by the South Australian government to ensure that South Australians can reap the maximum benefit of the shipbuilding program; and
-(c) notes the significant negative impacts on the current workforce as a result of the former federal Labor government's failure to progress any future shipbuilding contracts during its last term in office.
-The $90 billion shipbuilding program committed to by the federal Liberal government has been a landmark decision which will reap benefits for South Australia for many years to come. The decision will modernise and strengthen Australia's naval forces and will underpin employment, build workforce capacity, investment, innovation and experience in shipbuilding in Australia. In particular for South Australian investment, it will yield significant economic benefits. The investment will create significant supply chain growth opportunities which are in addition to the more than 5,000 direct jobs that will be created through naval shipbuilding activities in South Australia.
-The funding will enable the build of 12 Attack class submarines, which I am told is the largest defence procurement initiative in Australia's history. The funding will enable a $35 billion Hunter class frigate program, which will deliver nine antisubmarine frigates to the Royal Australian Navy and will create and sustain 1,500 direct jobs. This will be in addition to the 600 jobs needed for the redevelopment of the Osborne South Shipyard and provide opportunities through the supply chain. The supply chain benefits will be substantial. The new Lot Fourteen innovation neighbourhood will provide a location which will attract global companies to develop their Australian business strategy and plan local operations.
-A new one-stop shop, supporting international defence companies to establish in South Australia, will drive defence industry investment. The Defence Landing Pad at Lot Fourteen will enable international businesses to build relationships with South Australian businesses and create opportunities for supply chain collaboration. The investment by the federal Liberal government will assist in bridging the unemployment vacuum that was created by the previous federal Labor government's lack of vision. Unfortunately, it dropped the ball regarding Australia's shipbuilding industry and its workers.
-We know that in Osborne today the last program is winding up. I can tell you that there are still employees there today being told that their jobs are about to finish. The contract is now winding down and their jobs no longer exist until this shipbuilding operation is back up to speed, back on the build, where it should have been four or five years ago. We know that there are some employees being re-engaged down there, but they are not the same ones who have been told their job no longer exists because they have come to the end of that contract.
-It shows that if this is going to be managed—and not to play politics with this and say that one side of politics is better than the other—it will require a united front on both sides of politics to recognise this as a big build for Australia. If we work together on the fact that it needs to happen in a methodical way that looks after the federal government's interests, the state government's interests and those of employees, contractors and builders alike, then it can be an absolutely wonderful opportunity for Australia.
-To summarise, we know the new patrol boats are just starting off. I believe there are going to be two built in Adelaide to start off with, of the perhaps 12 that Australia will build. It is a starting point. They are employing people who start off by doing the groundwork, what we call laying down the keel. They will be building the bulkheads. There are no electricians yet. They are not mechanics, they are not chippies, they are not electricians or technologists with technical expertise, because they are not required right now. Those areas of expertise are not needed.
-This is where the vacuum and the lack of cohesion from one build to the next needs to be absolutely methodical and straightforward so that all employees in this region can have a job from one week to the next, one month to the next and one year to the next. This is so we can create consistent work in a consistent workplace where people can live their lives, build houses and dreams and know that this work will continue for many years to come.
-The ASC Shipbuilding Structural Adjustment Program, announced by the Australian government, will support workers who have been made redundant, and it will be backdated to 1 July 2018, because of the lack of foresight by our federal Labor government. I am advised that workers and their partners from ASC Shipbuilding or an affected supply chain business are also eligible for this program. The program will offer a range of services for employees both before their positions are discontinued and after. The types of services offered will include career advice, skills assessment and labour market information to assist people to make decisions on their next steps.
-The service will also include intensive employment support through Jobactive employment providers, job search support and retraining. This program will include a $2,000 employment fund to assist workers to retain and obtain licences and tickets, as well as relocation assistance if required. The investment by the federal Liberal government and the efforts of the Marshall Liberal government in continuous naval shipbuilding will create thousands of jobs for decades to come. There will be a period of supported transition as our current shipbuilding workforce redeploys to new opportunities being created across our defence industry base. Two of the offshore patrol boats are currently being built by ASC, with production directly employing up to 400 workers at Osborne and 600 indirectly.
-This gives me a bit of an opportunity to address the comments made by the member for Croydon (the Leader of the Opposition), who talked about the Collins class submarines and the history of Australian shipbuilding, as we know it so far. I do not want to play politics, but I want to make sure that our Liberal government recognises that it actually does take effort to ensure this will be a good and profitable build and one that builds a product that we can be proud of for many years to come.
-I note that the six Collins class submarines that were started in 1990 and finished in 2003 were costed at $4 billion to start off but blew out to $5.1 billion—27 per cent; $5 billion to $4 billion is not much. This is a $90 billion build, and if we blow out that budget by 27 per cent, that is an extra $24 billion that this one overall contract will cost if we do not do it properly. It will blow out to $117 billion on the same basis as the Collins class submarines.
-The opposition leader is worried about local content. Belonging to the Liberal Party government, I too want as much local content and build in South Australia as possible, but not at any cost, not at any blowout for many, many years beyond what it is meant to be. Absolutely, these boats have to work. There were six Collins class submarines. They only ever had, at some stage, a 35 per cent workforce working on the submarines because they were such high maintenance dependent. They were costing a fortune to maintain and operate. It was not just the worker base but also the fact that the Collins class submarine had huge issues of maintenance and standard.
-One of the biggest pitfalls, they tell me, is that we changed our mind during the build. The defence system wanted this and then they wanted that, and then it did not fit and then it did not work, and they would not talk each other. Technological advances were always on the go. One of the things that I hope we do with this large contract is to make sure that this build is a good fit, works for Australia's purposes, does not blow out and is not at any cost. This is unlike the Labor Party on the other side, which says: 'Just employ people, just spend money, just get jobs.' No, not at any cost at all.
-From my own history, having trained as a boilermaker/welder through an apprenticeship program, I am really excited about the investment the Marshall Liberal government is making to build the capacity and capability of South Australians. The program is going to yield a great many benefits for trade industries and it will provide opportunities for trainees. The more than 20,000 new apprenticeships and trainees that will be created have been made possible through the federal government's Skilling Australians Fund. They will offer really great opportunities for people to upskill and reskill in order to take advantage of new employment opportunities like this shipbuilding program.
-These positions will be supported by the establishment of a new technical college in Adelaide's western suburbs, with a focus on defence, and a range of other measures, including the re-establishment of industry skills councils to give industry a strong voice and a pathway to work, with government to strengthen and influence the vocational education training system. I commend the motion to the house.
-The Hon. Z.L. BETTISON (Ramsay) (12:03): I rise to speak on the amended motion. One of my motivations for being in politics was employment. When I finished school and university, it was really difficult to get a job. I had fantastic mentors. My parents both worked. They had a business, and they supported post secondary education. My concern today is this issue because when I am out doorknocking people ask me, 'What are the jobs of the future? What will my children do? What will my grandchildren do?' We know that we have a fantastic opportunity in South Australia with this shipbuilding program. We all agree that this is a wonderful opportunity.
-There are discussions that there will be up to 25,000 jobs in South Australia, so imagine my disappointment and my surprise that there is absolutely no commitment to local content. How do we expect our parents and grandparents to encourage their children to train in the areas that are going to be needed for this shipbuilding program?
-I acknowledge the Skilling Australia program and I acknowledge the Naval Shipbuilding College, but what we need to do is make all South Australians aware of what the jobs are and the pathways to get those jobs. Whether it be an electrician, a mechanic, a welder, a fitter and turner, like my own father when he did his apprenticeship, or be skills in technology or design, we know that those jobs are going to be needed.
-What we do not know is if those 25,000 proposed jobs are ever actually going to happen, because what we hear is the politics being played out. When we hear people being told in November 2017 that we are going to create 25,000 jobs in South Australia, and in December 2018 being assured by minister Pyne that these jobs will be delivered through an assured level of local content, that this will be a local build, that is what our parents and grandparents hear. 'Fantastic! This is what we are going to encourage our children to do.'
-We know that science, technology, engineering and mathematics are going to be crucial in taking up these jobs. I am excited about it. This is something that we can share. We can be part of world's best practice of this amazing advanced manufacturing. We welcome it; this is fantastic. But when we hear that there is no guarantee of local content, how can we say this to our South Australians? How can we encourage them to train in this sector? This is the concern that I raise with this issue today.
-What I am very concerned about is our Premier not standing up for our state. Sure, he might have been there for the signing, but where is his commitment, where is our understanding of the state government supporting, encouraging and knowing how many of these jobs there will be? That is why I rise today to support the amended motion.
-Mr PATTERSON (Morphett) (12:07): I rise to welcome the federal Liberal government's commitment to the $90 billion shipbuilding program that is centred in this state and to speak in support of the member for Colton's motion. We know that as the program to build air warfare destroyers at the Osborne naval shipbuilding precinct comes to an end, the federal government is now centring its naval shipbuilding program in South Australia, with the construction of the first two offshore patrol vessels, followed by the Future Frigate program and the submarine program.
-This $90 billion commitment will modernise and strengthen Australia's naval forces. We know that ASC has built up considerable skills over the last 10 years on the air warfare destroyer program, and the highly skilled shipbuilders, in conjunction with this new naval shipbuilding program, can be the basis for building a strong, sustainable sovereign Australian shipbuilding industry. It will certainly define the future of advanced manufacturing in Australia and it is happening right here in South Australia.
-These first two offshore patrol vessels are going to be constructed in South Australia by ASC and will overcome the valley of death between the end of the air warfare destroyer program and the beginning of the Future Frigate program. Unfortunately, prior to the commitment of the construction of these first two offshore patrol vessels at Osborne, the gap saw the steady release of the workforce and hence the loss of valuable skilled workers prior to the commencement of the Future Frigates shipbuilding program.
-It was therefore welcome news when in November 2018 work began on the first of these offshore patrol vessels at Osborne, with the welding of the first two component blocks of steel that will form part of the first vessel. The new ships will be known as the Arafura class, with the first to enter service in 2022 to be called the HMAS Arafura.
-The ASC chief executive noted </t>
-  </si>
-  <si>
     <t>Adjourned debate on second reading.
 (Continued from 16 May 2018.)
 The Hon. I. PNEVMATIKOS (16:54): Today I rise to speak on the Statutes Amendment (Decriminalisation of Sex Work) Bill (No. 2). This is a matter that has been debated many times in respect of how it should be governed. In fact, in the last 20 years there have been 12 bills introduced to decriminalise sex work and none of them has been successful. Why? Because it is a contentious issue, heavily cloaked in stigma. More oft than not, the moral values and personal beliefs of a few have drowned out the voices of the many and, in particular, those on the front line. Voices such as Scarlet Alliance, SIN, the World Health Organization and the workers themselves, who are willing to risk a great deal to be seen, heard and taken seriously.
@@ -757,11 +671,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1090,11 +1001,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E2EC93-960C-48F4-A506-84E0208EB621}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:G21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1107,7 +1018,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1116,379 +1027,360 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>43523</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>43677</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>43678</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>43523</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="6" t="s">
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>43621</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>43648</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
-        <v>43523</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>43677</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="F6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>43678</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>43621</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>43648</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="2">
+        <v>43712</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>43601</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>43712</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>43601</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>43601</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>43635</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>43601</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="6" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>43635</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>43508</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>43635</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="B13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
         <v>43635</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>43635</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>43440</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
         <v>43508</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>43635</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>43635</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>43635</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
-        <v>43440</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="6" t="s">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>43557</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="8">
+      <c r="F18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>43510</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
         <v>43508</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="8">
-        <v>43557</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="6" t="s">
+      <c r="B20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="8">
-        <v>43510</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
-        <v>43508</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" location="/docid/HANSARD-11-33034" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-33034" xr:uid="{CF7EEAFE-37A7-4A68-8BFC-83188235D4C6}"/>
-    <hyperlink ref="F3" r:id="rId2" location="/docid/HANSARD-10-26906" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26906" xr:uid="{E852C2AD-6FE3-4882-8137-43B1A4DF1244}"/>
-    <hyperlink ref="F4" r:id="rId3" location="/docid/HANSARD-11-34810" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-34810" xr:uid="{60BD940E-0B70-4EE5-AF87-1AE4F8251902}"/>
-    <hyperlink ref="F5" r:id="rId4" location="/docid/HANSARD-11-34872" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-34872" xr:uid="{52962164-55D7-4F46-B5FD-E6AA6DB58035}"/>
-    <hyperlink ref="F6" r:id="rId5" location="/docid/HANSARD-10-26904" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26904" xr:uid="{67034CF3-F99C-49AB-9556-C1D5087401F6}"/>
-    <hyperlink ref="F7" r:id="rId6" location="/docid/HANSARD-11-34466" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-34466" xr:uid="{0E91C013-3D9E-4F7D-85C5-A91B67C232EC}"/>
-    <hyperlink ref="F8" r:id="rId7" location="/docid/HANSARD-11-30661" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-30661" xr:uid="{702D05ED-05E6-461B-A612-AF73132F6FEC}"/>
-    <hyperlink ref="F9" r:id="rId8" location="/docid/HANSARD-10-26776" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26776" xr:uid="{717B5977-7B99-4BBA-8546-6F0293E2CB2D}"/>
-    <hyperlink ref="F10" r:id="rId9" location="/docid/HANSARD-11-33921" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-33921" xr:uid="{0FD9BB4C-B3CB-41B9-8B06-F3BAB6A7EE13}"/>
-    <hyperlink ref="F11" r:id="rId10" location="/docid/HANSARD-10-23279" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23279" xr:uid="{883ACBE4-87FE-43D8-84D9-D07334278DF1}"/>
-    <hyperlink ref="F12" r:id="rId11" location="/docid/HANSARD-10-23278" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23278" xr:uid="{73A3AD8E-5A9A-4FA9-AE35-3861574BB535}"/>
-    <hyperlink ref="F13" r:id="rId12" location="/docid/HANSARD-11-32755" xr:uid="{9BBE697E-7419-4F79-AC17-9A6ED5A7F9AF}"/>
-    <hyperlink ref="F14" r:id="rId13" location="/docid/HANSARD-10-23286" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23286" xr:uid="{D5E612D2-F917-4A06-A220-DA369BD0FC90}"/>
-    <hyperlink ref="F15" r:id="rId14" location="/docid/HANSARD-10-23290" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23290" xr:uid="{F6621F6B-BCEF-4586-AB26-109836F94128}"/>
-    <hyperlink ref="F16" r:id="rId15" location="/docid/HANSARD-10-23311" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23311" xr:uid="{955E183C-87B2-420F-85FD-B500A0537C06}"/>
-    <hyperlink ref="F17" r:id="rId16" location="/docid/HANSARD-11-32619" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-32619" xr:uid="{CDECA91D-9FCC-4506-9583-C5970EA4CDB6}"/>
-    <hyperlink ref="F18" r:id="rId17" location="/docid/HANSARD-11-32795" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-32795" xr:uid="{5142684D-AB52-459A-9453-7743A8F7BCF3}"/>
-    <hyperlink ref="F19" r:id="rId18" location="/docid/HANSARD-10-26307" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26307" xr:uid="{A6C8D112-203F-4AD7-BEA0-8C6AD9BDF709}"/>
-    <hyperlink ref="F20" r:id="rId19" location="/docid/HANSARD-11-32954" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-32954" xr:uid="{97BEC237-75A0-4245-A3E3-292074640C85}"/>
-    <hyperlink ref="F21" r:id="rId20" location="/docid/HANSARD-11-32797" display="/docid/HANSARD-11-32797" xr:uid="{3DAE44B1-0FA3-4B6D-98FA-56AF11AEE7FA}"/>
+    <hyperlink ref="F2" r:id="rId1" location="/docid/HANSARD-10-26906" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26906" xr:uid="{E852C2AD-6FE3-4882-8137-43B1A4DF1244}"/>
+    <hyperlink ref="F3" r:id="rId2" location="/docid/HANSARD-11-34810" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-34810" xr:uid="{60BD940E-0B70-4EE5-AF87-1AE4F8251902}"/>
+    <hyperlink ref="F4" r:id="rId3" location="/docid/HANSARD-11-34872" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-34872" xr:uid="{52962164-55D7-4F46-B5FD-E6AA6DB58035}"/>
+    <hyperlink ref="F5" r:id="rId4" location="/docid/HANSARD-10-26904" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26904" xr:uid="{67034CF3-F99C-49AB-9556-C1D5087401F6}"/>
+    <hyperlink ref="F6" r:id="rId5" location="/docid/HANSARD-11-34466" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-34466" xr:uid="{0E91C013-3D9E-4F7D-85C5-A91B67C232EC}"/>
+    <hyperlink ref="F7" r:id="rId6" location="/docid/HANSARD-11-30661" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-30661" xr:uid="{702D05ED-05E6-461B-A612-AF73132F6FEC}"/>
+    <hyperlink ref="F8" r:id="rId7" location="/docid/HANSARD-10-26776" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26776" xr:uid="{717B5977-7B99-4BBA-8546-6F0293E2CB2D}"/>
+    <hyperlink ref="F9" r:id="rId8" location="/docid/HANSARD-11-33921" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-33921" xr:uid="{0FD9BB4C-B3CB-41B9-8B06-F3BAB6A7EE13}"/>
+    <hyperlink ref="F10" r:id="rId9" location="/docid/HANSARD-10-23279" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23279" xr:uid="{883ACBE4-87FE-43D8-84D9-D07334278DF1}"/>
+    <hyperlink ref="F11" r:id="rId10" location="/docid/HANSARD-10-23278" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23278" xr:uid="{73A3AD8E-5A9A-4FA9-AE35-3861574BB535}"/>
+    <hyperlink ref="F12" r:id="rId11" location="/docid/HANSARD-11-32755" xr:uid="{9BBE697E-7419-4F79-AC17-9A6ED5A7F9AF}"/>
+    <hyperlink ref="F13" r:id="rId12" location="/docid/HANSARD-10-23286" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23286" xr:uid="{D5E612D2-F917-4A06-A220-DA369BD0FC90}"/>
+    <hyperlink ref="F14" r:id="rId13" location="/docid/HANSARD-10-23290" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23290" xr:uid="{F6621F6B-BCEF-4586-AB26-109836F94128}"/>
+    <hyperlink ref="F15" r:id="rId14" location="/docid/HANSARD-10-23311" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-23311" xr:uid="{955E183C-87B2-420F-85FD-B500A0537C06}"/>
+    <hyperlink ref="F16" r:id="rId15" location="/docid/HANSARD-11-32619" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-32619" xr:uid="{CDECA91D-9FCC-4506-9583-C5970EA4CDB6}"/>
+    <hyperlink ref="F17" r:id="rId16" location="/docid/HANSARD-11-32795" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-32795" xr:uid="{5142684D-AB52-459A-9453-7743A8F7BCF3}"/>
+    <hyperlink ref="F18" r:id="rId17" location="/docid/HANSARD-10-26307" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-10-26307" xr:uid="{A6C8D112-203F-4AD7-BEA0-8C6AD9BDF709}"/>
+    <hyperlink ref="F19" r:id="rId18" location="/docid/HANSARD-11-32954" display="http://hansardpublic.parliament.sa.gov.au/Pages/HansardResult.aspx - /docid/HANSARD-11-32954" xr:uid="{97BEC237-75A0-4245-A3E3-292074640C85}"/>
+    <hyperlink ref="F20" r:id="rId19" location="/docid/HANSARD-11-32797" display="/docid/HANSARD-11-32797" xr:uid="{3DAE44B1-0FA3-4B6D-98FA-56AF11AEE7FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>